<commit_message>
identified user email send
</commit_message>
<xml_diff>
--- a/django/clickserver/identified_user_activity_2023-07-24.xlsx
+++ b/django/clickserver/identified_user_activity_2023-07-24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,17 +485,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-07-02 23:42:10</t>
+          <t>2023-07-02</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "180555"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"| "visit_count": 7}| {"item__product_id": "173500"| "item__name": "hot pink embellished neck work cotton top with stripe printed chiffon dupatta set"| "visit_count": 5}| {"item__product_id": "182455"| "item__name": "Space Blue Chanderi Kantha 3 Piece Set"| "visit_count": 5}| {"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 5}| {"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"| "visit_count": 5}| {"item__product_id": "182300"| "item__name": "Nawabi Mint Green Authentic Chikankari Cotton Top with Cotton Dupatta Set"| "visit_count": 4}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"| "visit_count": 4}| {"item__product_id": "182279"| "item__name": "Kholapuri Beige Khadi Embroidered Cotton Top with Kota Dupatta Set"| "visit_count": 4}| {"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 4}| {"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"| "visit_count": 3}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"| "visit_count": 3}| {"item__product_id": "177150"| "item__name": "purple bandhani inspired printed cotton top"| "visit_count": 3}| {"item__product_id": "179104"| "item__name": "Sapphire Blue Floral Printed Cotton Top"| "visit_count": 3}| {"item__product_id": "182547"| "item__name": "Barbie Blue Leheriya Printed Lace Work Cotton Top"| "visit_count": 3}| {"item__product_id": "179908"| "item__name": "cinnamon brown cotton linen floral chikankari work kurti"| "visit_count": 3}| {"item__product_id": "182224"| "item__name": "Mahreen Light Orchid Candy Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 3}| {"item__product_id": "166662"| "item__name": "dove greyish purple printed chikankari top with leheriya printed palazzo"| "visit_count": 3}| {"item__product_id": "182698"| "item__name": "Nihari Sage Green Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 2}| {"item__product_id": "182439"| "item__name": "Mystic Mauvewood Chanderi Top with Hand Painted Chiffon Dupatta Set"| "visit_count": 2}| {"item__product_id": "159525"| "item__name": "light orange south cotton top with mangalgiri hem with barn red dupatta"| "visit_count": 2}| {"item__product_id": "172717"| "item__name": "black and white modal chikankari kurti"| "visit_count": 2}| {"item__product_id": "130755"| "item__name": "moss green printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 2}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"| "visit_count": 2}| {"item__product_id": "176295"| "item__name": "sapphire blue polka dot cotton top"| "visit_count": 2}| {"item__product_id": "178640"| "item__name": "Creamy White Printed Cotton Top and Teal Green Bottom with Cotton Dupatta Set"| "visit_count": 2}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "172317"| "item__name": "Off-white Patra Work Cotton Pakistani Suit with Chiffon Dupatta Set"| "visit_count": 2}| {"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"| "visit_count": 2}| {"item__product_id": "182195"| "item__name": "Lehar Salmon Peach Lace Work Leheriya Cotton Top With Semi Cotton and Organza Dupatta set"| "visit_count": 2}| {"item__product_id": "109151"| "item__name": "white applique scallop palazzo trouser"| "visit_count": 2}| {"item__product_id": "172287"| "item__name": "cream white crochet work pakistani suit with printed chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "170075"| "item__name": "light blue floral printed button down shirt"| "visit_count": 2}| {"item__product_id": "177963"| "item__name": "bright pink georgette leheriya top with leheriya chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "131381"| "item__name": "hot pink silk v neck top with banarasi dupatta set"| "visit_count": 2}| {"item__product_id": "177072"| "item__name": "Mushroom Grey Chanderi Embroidered Work Top and Dupatta Set"| "visit_count": 2}| {"item__product_id": "178930"| "item__name": "candy pink stripe jam cotton top with cotton dupatta set"| "visit_count": 2}| {"item__product_id": "171502"| "item__name": "maroon and grey shibori digital print cotton silk with shibori print dupatta set"| "visit_count": 2}| {"item__product_id": "182290"| "item__name": "Nawabi LiLac Authentic Chikankari Cotton Top with Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "166319"| "item__name": "light peach chikankari cotton linen top with schiffli bottom 2 piece set"| "visit_count": 1}| {"item__product_id": "149968"| "item__name": "Pearl White Cotton Schiffli Fabric- 2"| "visit_count": 1}| {"item__product_id": "180004"| "item__name": "cream white cotton top with neon pink patola print dupatta set"| "visit_count": 1}| {"item__product_id": "95820"| "item__name": "offwhite full schiffali work trouser"| "visit_count": 1}| {"item__product_id": "181159"| "item__name": "Denim blue Tussar Chanderi Dupatta"| "visit_count": 1}| {"item__product_id": "182854"| "item__name": "Cobalt Blue South Cotton Top with Mangalgiri Hem and Denim Blue Dupatta Set"| "visit_count": 1}| {"item__product_id": "182409"| "item__name": "Laffy Taffy Lavender Embellished Neck Work Organza Top with Organza Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182401"| "item__name": "Sizzler Baby Pink Authentic Bandhej Top with Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182389"| "item__name": "Zebra Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "182264"| "item__name": "Ribollita Baby Blue Digital Printed Glazed Cotton Top with Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "116991"| "item__name": "currant red bandhej cotton top with fire yellow dupatta set"| "visit_count": 1}| {"item__product_id": "180249"| "item__name": "Dandelion Yellow Glazed Cotton Printed Top with Glazed Cotton Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "166907"| "item__name": "lapis blue printed cotton top with bumblebee yellow chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "137784"| "item__name": "Fire Red Printed Chikankari Kurti"| "visit_count": 1}| {"item__product_id": "178922"| "item__name": "opera mauve thread work cotton top with printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "175168"| "item__name": "dark magenta chikankari georgette 3 piece set"| "visit_count": 1}| {"item__product_id": "157179"| "item__name": "lavender chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "172355"| "item__name": "antique mauve cross stitch work cotton linen top and dupatta set d2 2"| "visit_count": 1}| {"item__product_id": "160312"| "item__name": "rose pink authentic dabu printed top and dupatta set"| "visit_count": 1}| {"item__product_id": "177217"| "item__name": "mint green crochet work cotton top with hand printed chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "136410"| "item__name": "mint green printed cotton top and bottom with plain chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "180255"| "item__name": "Mint Green Glazed Glazed Cotton Printed Top with Glazed Cotton Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "181955"| "item__name": "Mint Green Digital Printed Cotton Linen Top and Dupatta Set-D2"| "visit_count": 1}| {"item__product_id": "170739"| "item__name": "winchester grey printed south cotton top with mangalgiri hem with black dupatta set"| "visit_count": 1}| {"item__product_id": "148835"| "item__name": "purple and orange printed top and dupatta set"| "visit_count": 1}| {"item__product_id": "181604"| "item__name": "Carolina Blue Printed Cotton Top with Cream Bottom and White Printed Kota Dupatta Set"| "visit_count": 1}| {"item__product_id": "181470"| "item__name": "Ivory White Plain Lycra Trouser with Lace"| "visit_count": 1}| {"item__product_id": "169185"| "item__name": "jade green crochet work pakistani suit with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "178956"| "item__name": "baby blue stripe jam cotton top with cotton dupatta set"| "visit_count": 1}| {"item__product_id": "181544"| "item__name": "Ivory White Floral Printed Muslin Kaftan"| "visit_count": 1}| {"item__product_id": "159102"| "item__name": "Raisin and Cream Printed Cotton Top with Cream Chiffon Hand Painted Dupatta Set"| "visit_count": 1}| {"item__product_id": "168581"| "item__name": "sage green digital printed muslin 3 piece set with beautiful lace work dupatta"| "visit_count": 1}| {"item__product_id": "167071"| "item__name": "rouge pink dabu work kantha cotton fabric with schiffli"| "visit_count": 1}| {"item__product_id": "180201"| "item__name": "Beige Ikkat Printed Khadi Cotton Top with Munsell Purple Dupatta Set"| "visit_count": 1}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"| "visit_count": 1}| {"item__product_id": "176269"| "item__name": "creamy pink floral printed cotton top"| "visit_count": 1}| {"item__product_id": "176296"| "item__name": "crimson pink v neck cotton flax top"| "visit_count": 1}| {"item__product_id": "176281"| "item__name": "salmon peach lace work cotton flax top"| "visit_count": 1}| {"item__product_id": "155230"| "item__name": "carrot pink embroidered kota top and dupatta 2 piece set"| "visit_count": 1}| {"item__product_id": "155223"| "item__name": "sky blue embroidered kota top and dupatta 2 piece set"| "visit_count": 1}| {"item__product_id": "166086"| "item__name": "grey chikankari cotton 2 piece set"| "visit_count": 1}| {"item__product_id": "155185"| "item__name": "peach embroidered kota top and dupatta 2 piece set"| "visit_count": 1}| {"item__product_id": "182144"| "item__name": "Bright Pink Leheriya Printed Cotton Top with Shibori Printed Cotton Dupatta Set (Copy)"| "visit_count": 1}| {"item__product_id": "182720"| "item__name": "Ghoomer Olive Yelllow Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182856"| "item__name": "Faded Brown South Cotton Top with Mangalgiri Hem with Dark Barn Red Dupatta"| "visit_count": 1}| {"item__product_id": "182677"| "item__name": "Ghoomer Brown Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182731"| "item__name": "Ruhi Mauve Pink Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182163"| "item__name": "Gulab Jamun Eggplant Georgette Top with Leheriya Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "112916"| "item__name": "french violet french knot top with white chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "172432"| "item__name": "creamy white embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "151028"| "item__name": "brown printed top with digital printed dupatta set"| "visit_count": 1}| {"item__product_id": "172175"| "item__name": "chestnut brown embroidered chanderi top with digital printed chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "179340"| "item__name": "maroon red chikankari work rayon top with palazzo"| "visit_count": 1}| {"item__product_id": "177935"| "item__name": "baby pink floral printed cotton top with hand printed kota dupatta set"| "visit_count": 1}| {"item__product_id": "182540"| "item__name": "Barbie Pink Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "172314"| "item__name": "cream white and purple crochet work pakistani suit with printed chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "151525"| "item__name": "charcoal grey modal chikankari kurti"| "visit_count": 1}| {"item__product_id": "138758"| "item__name": "charcoal grey self digital printed top and dupatta set 2"| "visit_count": 1}| {"item__product_id": "164830"| "item__name": "scarlet red ikkat cotton co ord set"| "visit_count": 1}| {"item__product_id": "156475"| "item__name": "black and pink printed cotton 3 piece set"| "visit_count": 1}| {"item__product_id": "176225"| "item__name": "pastel purple french knot detailing chanderi top with floral printed chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "142732"| "item__name": "Black and Pink Screen Printed 2 Piece Fabric"| "visit_count": 1}| {"item__product_id": "138194"| "item__name": "black and pink print on print 2 piece set"| "visit_count": 1}| {"item__product_id": "182408"| "item__name": "Sizzler Bright Yellow Authentic Bandhej Top with Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182438"| "item__name": "Champagne Dream Biege Embellished Neckline Chanderi Top with Leheriya Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "177177"| "item__name": "baby blue chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "182152"| "item__name": "Gulab Jamun Eggplant Georgette Leheriya Top with Leheriya Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "172385"| "item__name": "mustard yellow kantha cotton top with black ajrak printed dupatta set d2"| "visit_count": 1}| {"item__product_id": "182156"| "item__name": "Blissta Black Embellished Neck Work Silk Top With Banarasi Dupatta Set"| "visit_count": 1}| {"item__product_id": "147381"| "item__name": "light beige mughal printed cotton top and bottom with kota dupatta 3 piece set"| "visit_count": 1}| {"item__product_id": "137057"| "item__name": "light orchid candy stripe printed cotton top with kota hand painted dupatta set"| "visit_count": 1}| {"item__product_id": "175558"| "item__name": "buttermilk yellow digital printed floral chikankari kurti d2"| "visit_count": 1}| {"item__product_id": "174161"| "item__name": "cyan blue zari work v neck georgette top with floral printed organza dupatta set"| "visit_count": 1}| {"item__product_id": "178840"| "item__name": "turquoise blue batik handloom top with dupatta set d2"| "visit_count": 1}| {"item__product_id": "142733"| "item__name": "cobalt blue printed 2 piece fabric"| "visit_count": 1}| {"item__product_id": "143685"| "item__name": "Dark Blue Ajrak Inspired Printed Cotton Fabric- 1"| "visit_count": 1}| {"item__product_id": "181790"| "item__name": "Cobalt Blue Printed Cotton Fabric"| "visit_count": 1}| {"item__product_id": "181041"| "item__name": "Purplish Floral Printed Cotton fabric"| "visit_count": 1}| {"item__product_id": "175411"| "item__name": "neon green floral printed co ord set"| "visit_count": 1}| {"item__product_id": "177102"| "item__name": "pearl white angrakha style cotton kurti"| "visit_count": 1}| {"item__product_id": "145469"| "item__name": "white and pink floral printed cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "166933"| "item__name": "offwhite floral printed kurti with front buttons"| "visit_count": 1}| {"item__product_id": "175250"| "item__name": "butterscotch yellow modal short chikankari kurti"| "visit_count": 1}| {"item__product_id": "177181"| "item__name": "baby pink chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "179493"| "item__name": "Pastel Pink Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "179876"| "item__name": "ivory blue cotton linen floral chikankari work kurti"| "visit_count": 1}| {"item__product_id": "179898"| "item__name": "Tea Green Cotton Linen Floral Chikankari Work Kurti"| "visit_count": 1}| {"item__product_id": "179959"| "item__name": "ruby pink embellished neckline muslin top with chanderi silk dupatta set"| "visit_count": 1}| {"item__product_id": "97351"| "item__name": "maroon straight fit kurti"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "180555"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"| "visit_count": 11}| {"item__product_id": "182290"| "item__name": "Nawabi LiLac Authentic Chikankari Cotton Top with Cotton Dupatta Set"| "visit_count": 7}| {"item__product_id": "182300"| "item__name": "Nawabi Mint Green Authentic Chikankari Cotton Top with Cotton Dupatta Set"| "visit_count": 7}| {"item__product_id": "182455"| "item__name": "Space Blue Chanderi Kantha 3 Piece Set"| "visit_count": 7}| {"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 7}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"| "visit_count": 7}| {"item__product_id": "170426"| "item__name": "amber yellow cotton dobby top with stripe print dupatta set"| "visit_count": 6}| {"item__product_id": "164822"| "item__name": "mint green neck thread work kota doriya top and dupatta set"| "visit_count": 6}| {"item__product_id": "170419"| "item__name": "hot pink cotton dobby top with stripe print dupatta set"| "visit_count": 5}| {"item__product_id": "161155"| "item__name": "flamingo pink kota doriya thread work top with chiffon printed dupatta set"| "visit_count": 5}| {"item__product_id": "182339"| "item__name": "Mohini Light Mauve Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 5}| {"item__product_id": "179506"| "item__name": "Mellow Yellow Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 5}| {"item__product_id": "182749"| "item__name": "Mastani Purple V neck Printed Muslin Top With Thread Work Organza Dupatta Set"| "visit_count": 4}| {"item__product_id": "182224"| "item__name": "Mahreen Light Orchid Candy Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 4}| {"item__product_id": "172385"| "item__name": "mustard yellow kantha cotton top with black ajrak printed dupatta set d2"| "visit_count": 4}| {"item__product_id": "173500"| "item__name": "hot pink embellished neck work cotton top with stripe printed chiffon dupatta set"| "visit_count": 4}| {"item__product_id": "180557"| "item__name": "Mulberry Mauve Thread Work Cotton Top with Chanderi Silk Dupatta Set"| "visit_count": 4}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"| "visit_count": 4}| {"item__product_id": "182279"| "item__name": "Kholapuri Beige Khadi Embroidered Cotton Top with Kota Dupatta Set"| "visit_count": 4}| {"item__product_id": "166662"| "item__name": "dove greyish purple printed chikankari top with leheriya printed palazzo"| "visit_count": 4}| {"item__product_id": "183087"| "item__name": "Ivory South Cotton V Neck with Mangalgiri Hem with Midnight Blue Dupatta Set"| "visit_count": 3}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"| "visit_count": 3}| {"item__product_id": "162133"| "item__name": "sage green digital printed top with chiffon dupatta set"| "visit_count": 3}| {"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"| "visit_count": 3}| {"item__product_id": "181948"| "item__name": "Eggplant Purple Digital Printed Cotton Linen Top and Dupatta Set-D2"| "visit_count": 3}| {"item__product_id": "179502"| "item__name": "Blush Pink Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 3}| {"item__product_id": "172384"| "item__name": "maroon red kantha cotton top with rust red ajrak printed dupatta set d2"| "visit_count": 3}| {"item__product_id": "182264"| "item__name": "Ribollita Baby Blue Digital Printed Glazed Cotton Top with Organza Dupatta Set"| "visit_count": 3}| {"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"| "visit_count": 3}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"| "visit_count": 3}| {"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"| "visit_count": 3}| {"item__product_id": "177150"| "item__name": "purple bandhani inspired printed cotton top"| "visit_count": 3}| {"item__product_id": "179104"| "item__name": "Sapphire Blue Floral Printed Cotton Top"| "visit_count": 3}| {"item__product_id": "179908"| "item__name": "cinnamon brown cotton linen floral chikankari work kurti"| "visit_count": 3}| {"item__product_id": "106956"| "item__name": "sky blue floral printed cotton top with stripe bottom and plain chiffon dupatta"| "visit_count": 2}| {"item__product_id": "179507"| "item__name": "Aqua Blue Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 2}| {"item__product_id": "181955"| "item__name": "Mint Green Digital Printed Cotton Linen Top and Dupatta Set-D2"| "visit_count": 2}| {"item__product_id": "178784"| "item__name": "mehndi green stripe printed cotton top with floral mul cotton dupatta set"| "visit_count": 2}| {"item__product_id": "182439"| "item__name": "Mystic Mauvewood Chanderi Top with Hand Painted Chiffon Dupatta Set"| "visit_count": 2}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 2}| {"item__product_id": "159525"| "item__name": "light orange south cotton top with mangalgiri hem with barn red dupatta"| "visit_count": 2}| {"item__product_id": "175082"| "item__name": "light lilac modal chikankari kurti"| "visit_count": 2}| {"item__product_id": "130755"| "item__name": "moss green printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 2}| {"item__product_id": "176295"| "item__name": "sapphire blue polka dot cotton top"| "visit_count": 2}| {"item__product_id": "155230"| "item__name": "carrot pink embroidered kota top and dupatta 2 piece set"| "visit_count": 2}| {"item__product_id": "166933"| "item__name": "offwhite floral printed kurti with front buttons"| "visit_count": 2}| {"item__product_id": "182438"| "item__name": "Champagne Dream Biege Embellished Neckline Chanderi Top with Leheriya Printed Chiffon Dupatta Set"| "visit_count": 2}| {"item__product_id": "182720"| "item__name": "Ghoomer Olive Yelllow Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 2}| {"item__product_id": "178640"| "item__name": "Creamy White Printed Cotton Top and Teal Green Bottom with Cotton Dupatta Set"| "visit_count": 2}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "182163"| "item__name": "Gulab Jamun Eggplant Georgette Top with Leheriya Chiffon Dupatta Set"| "visit_count": 2}| {"item__product_id": "182152"| "item__name": "Gulab Jamun Eggplant Georgette Leheriya Top with Leheriya Chiffon Dupatta Set"| "visit_count": 2}| {"item__product_id": "182259"| "item__name": "Darling Mulberry Violet Thread Work Muslin Top with Thread Work Organza Dupatta Set"| "visit_count": 2}| {"item__product_id": "175158"| "item__name": "eggplant purple chikankari georgette 3 piece set"| "visit_count": 2}| {"item__product_id": "182691"| "item__name": "Nihari Mauve Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 2}| {"item__product_id": "131381"| "item__name": "hot pink silk v neck top with banarasi dupatta set"| "visit_count": 2}| {"item__product_id": "177072"| "item__name": "Mushroom Grey Chanderi Embroidered Work Top and Dupatta Set"| "visit_count": 2}| {"item__product_id": "178930"| "item__name": "candy pink stripe jam cotton top with cotton dupatta set"| "visit_count": 2}| {"item__product_id": "171502"| "item__name": "maroon and grey shibori digital print cotton silk with shibori print dupatta set"| "visit_count": 2}| {"item__product_id": "179876"| "item__name": "ivory blue cotton linen floral chikankari work kurti"| "visit_count": 2}| {"item__product_id": "179898"| "item__name": "Tea Green Cotton Linen Floral Chikankari Work Kurti"| "visit_count": 2}| {"item__product_id": "177946"| "item__name": "midnight black thread work chanderi top with organza dupatta set"| "visit_count": 1}| {"item__product_id": "172734"| "item__name": "lilac printed cotton schiffli kurti"| "visit_count": 1}| {"item__product_id": "176601"| "item__name": "ebony black sequin work chanderi top with floral printed chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "176206"| "item__name": "light blue floral printed cotton top with flex cotton co ord set"| "visit_count": 1}| {"item__product_id": "182540"| "item__name": "Barbie Pink Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "166319"| "item__name": "light peach chikankari cotton linen top with schiffli bottom 2 piece set"| "visit_count": 1}| {"item__product_id": "149968"| "item__name": "Pearl White Cotton Schiffli Fabric- 2"| "visit_count": 1}| {"item__product_id": "180004"| "item__name": "cream white cotton top with neon pink patola print dupatta set"| "visit_count": 1}| {"item__product_id": "95820"| "item__name": "offwhite full schiffali work trouser"| "visit_count": 1}| {"item__product_id": "181159"| "item__name": "Denim blue Tussar Chanderi Dupatta"| "visit_count": 1}| {"item__product_id": "182854"| "item__name": "Cobalt Blue South Cotton Top with Mangalgiri Hem and Denim Blue Dupatta Set"| "visit_count": 1}| {"item__product_id": "175054"| "item__name": "blue mix color printed cotton chikankari kurti"| "visit_count": 1}| {"item__product_id": "177437"| "item__name": "black plain cotton flex trouser"| "visit_count": 1}| {"item__product_id": "169215"| "item__name": "periwinkle purple floral muslin top with cotton silk dupatta set"| "visit_count": 1}| {"item__product_id": "179919"| "item__name": "indigo printed v neck cotton top with printed bottom and dupatta set"| "visit_count": 1}| {"item__product_id": "168327"| "item__name": "sandcastle beige digital printed floral cotton linen top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "182698"| "item__name": "Nihari Sage Green Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 1}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182401"| "item__name": "Sizzler Baby Pink Authentic Bandhej Top with Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182389"| "item__name": "Zebra Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "116991"| "item__name": "currant red bandhej cotton top with fire yellow dupatta set"| "visit_count": 1}| {"item__product_id": "180249"| "item__name": "Dandelion Yellow Glazed Cotton Printed Top with Glazed Cotton Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "166907"| "item__name": "lapis blue printed cotton top with bumblebee yellow chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "137784"| "item__name": "Fire Red Printed Chikankari Kurti"| "visit_count": 1}| {"item__product_id": "178922"| "item__name": "opera mauve thread work cotton top with printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "181868"| "item__name": "Dark Pink and Magenta South Cotton Top with Mangalgiri Hem and Dupatta Set"| "visit_count": 1}| {"item__product_id": "176605"| "item__name": "cream white sequin work chanderi top with floral printed chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "131289"| "item__name": "tuscan sun yellow printed cotton top with tie and dye dupatta set"| "visit_count": 1}| {"item__product_id": "178923"| "item__name": "celadon blue thread work cotton top with printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "152076"| "item__name": "Salmon Peach Candy Stripe Printed Cotton Top with Kota Hand Painted Dupatta Set"| "visit_count": 1}| {"item__product_id": "177950"| "item__name": "Light Grey Floral Printed Cotton Top With Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}| {"item__product_id": "175168"| "item__name": "dark magenta chikankari georgette 3 piece set"| "visit_count": 1}| {"item__product_id": "157179"| "item__name": "lavender chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "172355"| "item__name": "antique mauve cross stitch work cotton linen top and dupatta set d2 2"| "visit_count": 1}| {"item__product_id": "160312"| "item__name": "rose pink authentic dabu printed top and dupatta set"| "visit_count": 1}| {"item__product_id": "177217"| "item__name": "mint green crochet work cotton top with hand printed chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "136410"| "item__name": "mint green printed cotton top and bottom with plain chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "180255"| "item__name": "Mint Green Glazed Glazed Cotton Printed Top with Glazed Cotton Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "170739"| "item__name": "winchester grey printed south cotton top with mangalgiri hem with black dupatta set"| "visit_count": 1}| {"item__product_id": "148835"| "item__name": "purple and orange printed top and dupatta set"| "visit_count": 1}| {"item__product_id": "181604"| "item__name": "Carolina Blue Printed Cotton Top with Cream Bottom and White Printed Kota Dupatta Set"| "visit_count": 1}| {"item__product_id": "181470"| "item__name": "Ivory White Plain Lycra Trouser with Lace"| "visit_count": 1}| {"item__product_id": "169185"| "item__name": "jade green crochet work pakistani suit with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "178956"| "item__name": "baby blue stripe jam cotton top with cotton dupatta set"| "visit_count": 1}| {"item__product_id": "169842"| "item__name": "sapphire blue printed cotton co ord set"| "visit_count": 1}| {"item__product_id": "172717"| "item__name": "black and white modal chikankari kurti"| "visit_count": 1}| {"item__product_id": "181544"| "item__name": "Ivory White Floral Printed Muslin Kaftan"| "visit_count": 1}| {"item__product_id": "159102"| "item__name": "Raisin and Cream Printed Cotton Top with Cream Chiffon Hand Painted Dupatta Set"| "visit_count": 1}| {"item__product_id": "168581"| "item__name": "sage green digital printed muslin 3 piece set with beautiful lace work dupatta"| "visit_count": 1}| {"item__product_id": "167071"| "item__name": "rouge pink dabu work kantha cotton fabric with schiffli"| "visit_count": 1}| {"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "180201"| "item__name": "Beige Ikkat Printed Khadi Cotton Top with Munsell Purple Dupatta Set"| "visit_count": 1}| {"item__product_id": "176269"| "item__name": "creamy pink floral printed cotton top"| "visit_count": 1}| {"item__product_id": "176296"| "item__name": "crimson pink v neck cotton flax top"| "visit_count": 1}| {"item__product_id": "176281"| "item__name": "salmon peach lace work cotton flax top"| "visit_count": 1}| {"item__product_id": "155223"| "item__name": "sky blue embroidered kota top and dupatta 2 piece set"| "visit_count": 1}| {"item__product_id": "166086"| "item__name": "grey chikankari cotton 2 piece set"| "visit_count": 1}| {"item__product_id": "155185"| "item__name": "peach embroidered kota top and dupatta 2 piece set"| "visit_count": 1}| {"item__product_id": "182686"| "item__name": "Ruhi Mehendi Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182144"| "item__name": "Bright Pink Leheriya Printed Cotton Top with Shibori Printed Cotton Dupatta Set (Copy)"| "visit_count": 1}| {"item__product_id": "182856"| "item__name": "Faded Brown South Cotton Top with Mangalgiri Hem with Dark Barn Red Dupatta"| "visit_count": 1}| {"item__product_id": "182677"| "item__name": "Ghoomer Brown Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182731"| "item__name": "Ruhi Mauve Pink Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182408"| "item__name": "Sizzler Bright Yellow Authentic Bandhej Top with Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182195"| "item__name": "Lehar Salmon Peach Lace Work Leheriya Cotton Top With Semi Cotton and Organza Dupatta set"| "visit_count": 1}| {"item__product_id": "177177"| "item__name": "baby blue chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "182156"| "item__name": "Blissta Black Embellished Neck Work Silk Top With Banarasi Dupatta Set"| "visit_count": 1}| {"item__product_id": "177963"| "item__name": "bright pink georgette leheriya top with leheriya chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "147381"| "item__name": "light beige mughal printed cotton top and bottom with kota dupatta 3 piece set"| "visit_count": 1}| {"item__product_id": "137057"| "item__name": "light orchid candy stripe printed cotton top with kota hand painted dupatta set"| "visit_count": 1}| {"item__product_id": "175558"| "item__name": "buttermilk yellow digital printed floral chikankari kurti d2"| "visit_count": 1}| {"item__product_id": "174161"| "item__name": "cyan blue zari work v neck georgette top with floral printed organza dupatta set"| "visit_count": 1}| {"item__product_id": "171041"| "item__name": "smokey purple floral muslin printed top and dupatta set"| "visit_count": 1}| {"item__product_id": "149638"| "item__name": "jade blue shade south cotton top with denim blue dupatta"| "visit_count": 1}| {"item__product_id": "152328"| "item__name": "grey base pink printed cotton chikankari 2 piece set"| "visit_count": 1}| {"item__product_id": "174871"| "item__name": "grapefruit purple printed chikankari top with leheriya printed palazzo"| "visit_count": 1}| {"item__product_id": "177856"| "item__name": "laurel green digital printed cotton linen top with cotton linen dupatta set"| "visit_count": 1}| {"item__product_id": "136467"| "item__name": "Mustard Yellow Kantha Cotton Top with Rust Red Ajrak Printed Dupatta 3 Piece Set"| "visit_count": 1}| {"item__product_id": "183059"| "item__name": "Ada Moss Brown Floral Printed Muslin Top with Thread Work Cotton Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "170838"| "item__name": "cyber yellow thread work chanderi top with organza dupatta set"| "visit_count": 1}| {"item__product_id": "173681"| "item__name": "peach embellished neck work zig zag muslin top with plain muslin dupatta set"| "visit_count": 1}| {"item__product_id": "177979"| "item__name": "maroon red embellished neck work muslin top with zari work chanderi silk dupatta set"| "visit_count": 1}| {"item__product_id": "182375"| "item__name": "Leher Violet Purple Cotton Leheriya Top with Shibori Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "177935"| "item__name": "baby pink floral printed cotton top with hand printed kota dupatta set"| "visit_count": 1}| {"item__product_id": "182355"| "item__name": "Mohini Beige White Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}| {"item__product_id": "183016"| "item__name": "Lahori Jade Green Cotton Pakistani Suit with Embroidered Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "180386"| "item__name": "Maroon Kalamkari Printed Cotton Top with Dobby Work Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "177102"| "item__name": "pearl white angrakha style cotton kurti"| "visit_count": 1}| {"item__product_id": "145469"| "item__name": "white and pink floral printed cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "175250"| "item__name": "butterscotch yellow modal short chikankari kurti"| "visit_count": 1}| {"item__product_id": "177181"| "item__name": "baby pink chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "179493"| "item__name": "Pastel Pink Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "179959"| "item__name": "ruby pink embellished neckline muslin top with chanderi silk dupatta set"| "visit_count": 1}| {"item__product_id": "97351"| "item__name": "maroon straight fit kurti"| "visit_count": 1}| {"item__product_id": "117527"| "item__name": "crimson pink muslin 3 piece garara set"| "visit_count": 1}| {"item__product_id": "109151"| "item__name": "white applique scallop palazzo trouser"| "visit_count": 1}| {"item__product_id": "181409"| "item__name": "Maroon Wine Embroidered Glazed Cotton fabric"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "178956"| "item__name": "baby blue stripe jam cotton top with cotton dupatta set"}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"}| {"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"}| {"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"}| {"item__product_id": "176269"| "item__name": "creamy pink floral printed cotton top"}| {"item__product_id": "155230"| "item__name": "carrot pink embroidered kota top and dupatta 2 piece set"}| {"item__product_id": "180555"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"}| {"item__product_id": "180555"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"}| {"item__product_id": "176296"| "item__name": "crimson pink v neck cotton flax top"}| {"item__product_id": "176296"| "item__name": "crimson pink v neck cotton flax top"}| {"item__product_id": "179104"| "item__name": "Sapphire Blue Floral Printed Cotton Top"}| {"item__product_id": "176281"| "item__name": "salmon peach lace work cotton flax top"}| {"item__product_id": "176281"| "item__name": "salmon peach lace work cotton flax top"}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"}| {"item__product_id": "182540"| "item__name": "Barbie Pink Leheriya Printed Lace Work Cotton Top"}| {"item__product_id": "170075"| "item__name": "light blue floral printed button down shirt"}| {"item__product_id": "176225"| "item__name": "pastel purple french knot detailing chanderi top with floral printed chanderi dupatta set"}| {"item__product_id": "176225"| "item__name": "pastel purple french knot detailing chanderi top with floral printed chanderi dupatta set"}| {"item__product_id": "176225"| "item__name": "pastel purple french knot detailing chanderi top with floral printed chanderi dupatta set"}| {"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"}| {"item__product_id": "166662"| "item__name": "dove greyish purple printed chikankari top with leheriya printed palazzo"}| {"item__product_id": "182455"| "item__name": "Space Blue Chanderi Kantha 3 Piece Set"}| {"item__product_id": "145469"| "item__name": "white and pink floral printed cotton top and dupatta set"}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"}| {"item__product_id": "178930"| "item__name": "candy pink stripe jam cotton top with cotton dupatta set"}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"}| {"item__product_id": "179876"| "item__name": "ivory blue cotton linen floral chikankari work kurti"}| {"item__product_id": "179876"| "item__name": "ivory blue cotton linen floral chikankari work kurti"}| {"item__product_id": "179876"| "item__name": "ivory blue cotton linen floral chikankari work kurti"}]</t>
+          <t>[{"item__product_id": "178956"| "item__name": "baby blue stripe jam cotton top with cotton dupatta set"}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"}| {"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"}| {"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"}| {"item__product_id": "176269"| "item__name": "creamy pink floral printed cotton top"}| {"item__product_id": "155230"| "item__name": "carrot pink embroidered kota top and dupatta 2 piece set"}| {"item__product_id": "180555"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"}| {"item__product_id": "180555"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"}| {"item__product_id": "176296"| "item__name": "crimson pink v neck cotton flax top"}| {"item__product_id": "176296"| "item__name": "crimson pink v neck cotton flax top"}| {"item__product_id": "179104"| "item__name": "Sapphire Blue Floral Printed Cotton Top"}| {"item__product_id": "176281"| "item__name": "salmon peach lace work cotton flax top"}| {"item__product_id": "176281"| "item__name": "salmon peach lace work cotton flax top"}| {"item__product_id": "176269"| "item__name": "creamy pink floral printed cotton top"}| {"item__product_id": "176269"| "item__name": "creamy pink floral printed cotton top"}| {"item__product_id": "176269"| "item__name": "creamy pink floral printed cotton top"}| {"item__product_id": "155230"| "item__name": "carrot pink embroidered kota top and dupatta 2 piece set"}| {"item__product_id": "155230"| "item__name": "carrot pink embroidered kota top and dupatta 2 piece set"}| {"item__product_id": "155230"| "item__name": "carrot pink embroidered kota top and dupatta 2 piece set"}| {"item__product_id": "155230"| "item__name": "carrot pink embroidered kota top and dupatta 2 piece set"}| {"item__product_id": "155230"| "item__name": "carrot pink embroidered kota top and dupatta 2 piece set"}| {"item__product_id": "155223"| "item__name": "sky blue embroidered kota top and dupatta 2 piece set"}| {"item__product_id": "155185"| "item__name": "peach embroidered kota top and dupatta 2 piece set"}| {"item__product_id": "166933"| "item__name": "offwhite floral printed kurti with front buttons"}| {"item__product_id": "180557"| "item__name": "Mulberry Mauve Thread Work Cotton Top with Chanderi Silk Dupatta Set"}| {"item__product_id": "183087"| "item__name": "Ivory South Cotton V Neck with Mangalgiri Hem with Midnight Blue Dupatta Set"}| {"item__product_id": "183087"| "item__name": "Ivory South Cotton V Neck with Mangalgiri Hem with Midnight Blue Dupatta Set"}| {"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"}| {"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"}| {"item__product_id": "179507"| "item__name": "Aqua Blue Thread Work Chanderi Top with Printed Organza Dupatta Set"}| {"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"}| {"item__product_id": "171041"| "item__name": "smokey purple floral muslin printed top and dupatta set"}| {"item__product_id": "182224"| "item__name": "Mahreen Light Orchid Candy Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"}| {"item__product_id": "182264"| "item__name": "Ribollita Baby Blue Digital Printed Glazed Cotton Top with Organza Dupatta Set"}| {"item__product_id": "166662"| "item__name": "dove greyish purple printed chikankari top with leheriya printed palazzo"}| {"item__product_id": "182455"| "item__name": "Space Blue Chanderi Kantha 3 Piece Set"}| {"item__product_id": "145469"| "item__name": "white and pink floral printed cotton top and dupatta set"}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"}| {"item__product_id": "178930"| "item__name": "candy pink stripe jam cotton top with cotton dupatta set"}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"}| {"item__product_id": "179876"| "item__name": "ivory blue cotton linen floral chikankari work kurti"}| {"item__product_id": "179876"| "item__name": "ivory blue cotton linen floral chikankari work kurti"}| {"item__product_id": "179876"| "item__name": "ivory blue cotton linen floral chikankari work kurti"}| {"item__product_id": "166662"| "item__name": "dove greyish purple printed chikankari top with leheriya printed palazzo"}]</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-07-02 23:44:11</t>
+          <t>2023-07-02</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -533,22 +533,22 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>bangiarashmi</t>
+          <t>suman.lata</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3744</t>
+          <t>4812</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-07-03 02:32:17</t>
+          <t>2023-07-02</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "170097"| "item__name": "sepia brown and white printed cotton top with stripe printed dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "183087"| "item__name": "Ivory South Cotton V Neck with Mangalgiri Hem with Midnight Blue Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -562,22 +562,22 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>shikha.gupta</t>
+          <t>bangiarashmi</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1280</t>
+          <t>3744</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-07-03 08:18:26</t>
+          <t>2023-07-03</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "130483"| "item__name": "cranberry bandhej dola silk top and dupatta"| "visit_count": 1}| {"item__product_id": "177222"| "item__name": "bright pink bhandhej printed embellished neckline organza top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "119157"| "item__name": "raisin purple dola silk 3 piece set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "170097"| "item__name": "sepia brown and white printed cotton top with stripe printed dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -591,22 +591,22 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>niharika.chinnari</t>
+          <t>shikha.gupta</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>1280</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-07-03 11:07:37</t>
+          <t>2023-07-03</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177188"| "item__name": "pastel green chikankari work cotton top and dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "119157"| "item__name": "raisin purple dola silk 3 piece set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -620,27 +620,27 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>richa.bharti</t>
+          <t>shahanaglitz</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>6117</t>
+          <t>5871</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-07-03 11:52:09</t>
+          <t>2023-07-03</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "168415"| "item__name": "spanish orange modal chikankari kurti d1"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "178806"| "item__name": "canary yellow stripe printed cotton top with floral mul cotton dupatta set"| "visit_count": 1}| {"item__product_id": "180403"| "item__name": "Jam Red Applique Work Glazed Cotton Top with Art Chanderi Dupatta Set"| "visit_count": 1}| {"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "182037"| "item__name": "Ruhani Red Dark Green Ajrak Printed Cotton Top With Block Printed Kota Dupatta Set"| "visit_count": 1}| {"item__product_id": "172312"| "item__name": "shades of blue and green cotton pakistani suits with digital printed chiffon dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"}]</t>
         </is>
       </c>
     </row>
@@ -649,22 +649,22 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>nilima.kumari</t>
+          <t>niharika.chinnari</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>6372</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-07-03 15:10:38</t>
+          <t>2023-07-03</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182408"| "item__name": "Sizzler Bright Yellow Authentic Bandhej Top with Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "177188"| "item__name": "pastel green chikankari work cotton top and dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -678,109 +678,109 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
+          <t>richa.bharti</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>6117</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2023-07-03</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "168415"| "item__name": "spanish orange modal chikankari kurti d1"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>aarti.kapoor</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2023-07-03</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "182962"| "item__name": "Barbie World Pink French Knot Cotton Top with Chiffon Dupatta Set"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>dr apeksha.bhamare</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>6403</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2023-07-03 15:33:06</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-07-03</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>[{"item__product_id": "152231"| "item__name": "navy blue straight fit kurti"| "visit_count": 1}| {"item__product_id": "170868"| "item__name": "flamingo pink embroidered linen top with bird embroidered linen dupatta set"| "visit_count": 1}| {"item__product_id": "181409"| "item__name": "Maroon Wine Embroidered Glazed Cotton fabric"| "visit_count": 1}]</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Archana rana</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>7819967859</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2023-07-08 19:43:32</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>[{"item__product_id": "179534"| "item__name": "light teal blue chanderi top and all over aari work chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "176593"| "item__name": "sangria floral printed cotton linen with cotton linen dupatta set"| "visit_count": 1}| {"item__product_id": "179954"| "item__name": "cream white cotton top with royal blue chiffon dupatta set"| "visit_count": 1}]</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Ayesha Sultana</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>9845608474</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2023-07-09 11:54:21</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>[{"item__product_id": "180547"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"| "visit_count": 1}| {"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"| "visit_count": 1}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "177181"| "item__name": "baby pink chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"| "visit_count": 1}]</t>
-        </is>
-      </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Suvasree Nandy</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>9903321166</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>seema.choudhary</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6446</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-07-09 20:27:28</t>
+          <t>2023-07-03</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "140938"| "item__name": "light peach silk top with embellished neck line and banarasi dupatta set"| "visit_count": 1}| {"item__product_id": "170868"| "item__name": "flamingo pink embroidered linen top with bird embroidered linen dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "162223"| "item__name": "cobalt blue step leheriya chikankari kurti"| "visit_count": 1}| {"item__product_id": "179507"| "item__name": "Aqua Blue Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "170425"| "item__name": "shamrock green cotton dobby top with stripe print dupatta set"| "visit_count": 1}| {"item__product_id": "176359"| "item__name": "pearl white french knot cotton top with purple authentic french knot dupatta set d2"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -792,24 +792,24 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Poonam Krishna</t>
+          <t>Archana rana</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>8427180729</t>
+          <t>7819967859</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-07-10 10:15:56</t>
+          <t>2023-07-08</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "148339"| "item__name": "yellow and offwhite printed cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "145469"| "item__name": "white and pink floral printed cotton top and dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "179534"| "item__name": "light teal blue chanderi top and all over aari work chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "176593"| "item__name": "sangria floral printed cotton linen with cotton linen dupatta set"| "visit_count": 1}| {"item__product_id": "179954"| "item__name": "cream white cotton top with royal blue chiffon dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -821,82 +821,82 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2354323</t>
+          <t>Ayesha Sultana</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>53432343</t>
+          <t>9845608474</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-07-10 10:44:13</t>
+          <t>2023-07-09</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177072"| "item__name": "Mushroom Grey Chanderi Embroidered Work Top and Dupatta Set"| "visit_count": 2}]</t>
+          <t>[{"item__product_id": "180547"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"| "visit_count": 1}| {"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"| "visit_count": 1}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "177181"| "item__name": "baby pink chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}]</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>ayesha.sultana</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>6522</t>
-        </is>
-      </c>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Alka trivedi</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>9968400589</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2023-07-11 06:43:05</t>
+          <t>2023-07-09</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "180547"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"| "visit_count": 1}| {"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"| "visit_count": 1}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "177181"| "item__name": "baby pink chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "172433"| "item__name": "hazel wood beige embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Durga Gulmohar</t>
+          <t xml:space="preserve">Ritu shroff </t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>7701837561</t>
+          <t>9893973033</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2023-07-11 12:54:49</t>
+          <t>2023-07-09</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "161557"| "item__name": "beige and yellow digital printed linen top with chiffon dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "167074"| "item__name": "indigo dabu work kantha cotton fabric with schiffali fabric"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -908,24 +908,24 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C. S. Parulekar</t>
+          <t>Sunitha manoj Vora</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>7767031974</t>
+          <t>9840984168</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2023-07-11 16:22:16</t>
+          <t>2023-07-10</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "143242"| "item__name": "cadium green printed cotton fabric"| "visit_count": 1}| {"item__product_id": "182439"| "item__name": "Mystic Mauvewood Chanderi Top with Hand Painted Chiffon Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "178152"| "item__name": "Bumblebee Yellow Floral V Neck Muslin Top With Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "182996"| "item__name": "Lahori Shades of Blue and Green Cotton Pakistani Suits with Digital Printed Chiffon Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -937,53 +937,53 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Shalu</t>
+          <t>Poonam Krishna</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7879157127</t>
+          <t>8427180729</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2023-07-12 15:46:13</t>
+          <t>2023-07-10</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182722"| "item__name": "Ghoomer Moss Green Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 6}| {"item__product_id": "176593"| "item__name": "sangria floral printed cotton linen with cotton linen dupatta set"| "visit_count": 2}| {"item__product_id": "182699"| "item__name": "Nihari Bluish Grey Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 1}| {"item__product_id": "177857"| "item__name": "dusty mauve digital printed cotton linen top with cotton linen dupatta set"| "visit_count": 1}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"| "visit_count": 1}| {"item__product_id": "182455"| "item__name": "Space Blue Chanderi Kantha 3 Piece Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "148339"| "item__name": "yellow and offwhite printed cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "145469"| "item__name": "white and pink floral printed cotton top and dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182722"| "item__name": "Ghoomer Moss Green Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"}| {"item__product_id": "182455"| "item__name": "Space Blue Chanderi Kantha 3 Piece Set"}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Sumitha Sivadas K</t>
+          <t>2354323</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>9446141233</t>
+          <t>53432343</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2023-07-12 22:37:45</t>
+          <t>2023-07-10</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "178585"| "item__name": "Cyan Blue Authentic Chikankari Cotton Top with Chiffon Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "177072"| "item__name": "Mushroom Grey Chanderi Embroidered Work Top and Dupatta Set"| "visit_count": 2}| {"item__product_id": "175158"| "item__name": "eggplant purple chikankari georgette 3 piece set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -995,58 +995,58 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Ruchi Aggarwal</t>
+          <t>Shalini Dewan</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>9310278584</t>
+          <t>9914015426</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2023-07-13 09:19:07</t>
+          <t>2023-07-10</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "61618"| "item__name": "Red kurti with beige palazzo set"| "visit_count": 1}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "181604"| "item__name": "Carolina Blue Printed Cotton Top with Cream Bottom and White Printed Kota Dupatta Set"| "visit_count": 1}| {"item__product_id": "183077"| "item__name": "Mughal White with Lavender Printed Angrakha Cotton Top with Dual Shade Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182720"| "item__name": "Ghoomer Olive Yelllow Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "181604"| "item__name": "Carolina Blue Printed Cotton Top with Cream Bottom and White Printed Kota Dupatta Set"}| {"item__product_id": "181604"| "item__name": "Carolina Blue Printed Cotton Top with Cream Bottom and White Printed Kota Dupatta Set"}]</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Seema sachin punia </t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>9896229484</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ayesha.sultana</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>6522</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2023-07-13 09:43:18</t>
+          <t>2023-07-11</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 1}| {"item__product_id": "104294"| "item__name": "black mushru 3 piece set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "180547"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"| "visit_count": 1}| {"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"| "visit_count": 1}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "177181"| "item__name": "baby pink chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"}]</t>
         </is>
       </c>
     </row>
@@ -1055,134 +1055,138 @@
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Ranjith</t>
+          <t>jruchi82</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>5749</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2023-07-13 13:41:10</t>
+          <t>2023-07-11</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "180555"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"| "visit_count": 5}| {"item__product_id": "116991"| "item__name": "currant red bandhej cotton top with fire yellow dupatta set"| "visit_count": 1}| {"item__product_id": "182148"| "item__name": "Kesariya Bright Red Georgette Leheriya Top with Leheriya Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "166415"| "item__name": "cream and blue cotton dobby chikankari kurti"| "visit_count": 1}| {"item__product_id": "178956"| "item__name": "baby blue stripe jam cotton top with cotton dupatta set"| "visit_count": 1}| {"item__product_id": "169185"| "item__name": "jade green crochet work pakistani suit with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "181470"| "item__name": "Ivory White Plain Lycra Trouser with Lace"| "visit_count": 1}| {"item__product_id": "181604"| "item__name": "Carolina Blue Printed Cotton Top with Cream Bottom and White Printed Kota Dupatta Set"| "visit_count": 1}| {"item__product_id": "148835"| "item__name": "purple and orange printed top and dupatta set"| "visit_count": 1}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"| "visit_count": 1}| {"item__product_id": "173500"| "item__name": "hot pink embellished neck work cotton top with stripe printed chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "178922"| "item__name": "opera mauve thread work cotton top with printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "182439"| "item__name": "Mystic Mauvewood Chanderi Top with Hand Painted Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "137784"| "item__name": "Fire Red Printed Chikankari Kurti"| "visit_count": 1}| {"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "166907"| "item__name": "lapis blue printed cotton top with bumblebee yellow chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "180249"| "item__name": "Dandelion Yellow Glazed Cotton Printed Top with Glazed Cotton Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "182264"| "item__name": "Ribollita Baby Blue Digital Printed Glazed Cotton Top with Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "182389"| "item__name": "Zebra Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "182401"| "item__name": "Sizzler Baby Pink Authentic Bandhej Top with Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182698"| "item__name": "Nihari Sage Green Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 1}| {"item__product_id": "182409"| "item__name": "Laffy Taffy Lavender Embellished Neck Work Organza Top with Organza Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "182854"| "item__name": "Cobalt Blue South Cotton Top with Mangalgiri Hem and Denim Blue Dupatta Set"| "visit_count": 1}| {"item__product_id": "181159"| "item__name": "Denim blue Tussar Chanderi Dupatta"| "visit_count": 1}| {"item__product_id": "95820"| "item__name": "offwhite full schiffali work trouser"| "visit_count": 1}| {"item__product_id": "180004"| "item__name": "cream white cotton top with neon pink patola print dupatta set"| "visit_count": 1}| {"item__product_id": "149968"| "item__name": "Pearl White Cotton Schiffli Fabric- 2"| "visit_count": 1}| {"item__product_id": "166319"| "item__name": "light peach chikankari cotton linen top with schiffli bottom 2 piece set"| "visit_count": 1}| {"item__product_id": "182300"| "item__name": "Nawabi Mint Green Authentic Chikankari Cotton Top with Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182290"| "item__name": "Nawabi LiLac Authentic Chikankari Cotton Top with Cotton Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "169710"| "item__name": "burgundy digital printed top with kantha dupatta set"| "visit_count": 1}| {"item__product_id": "182722"| "item__name": "Ghoomer Moss Green Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182697"| "item__name": "Nihari Turkish Blue Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "178956"| "item__name": "baby blue stripe jam cotton top with cotton dupatta set"}]</t>
+          <t>[{"item__product_id": "169710"| "item__name": "burgundy digital printed top with kantha dupatta set"}| {"item__product_id": "182722"| "item__name": "Ghoomer Moss Green Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"}| {"item__product_id": "182697"| "item__name": "Nihari Turkish Blue Chanderi Silk Top with Printed Organza  Dupatta Set"}]</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Vandana Kone</t>
+          <t>Durga Gulmohar</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>9443887671</t>
+          <t>7701837561</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2023-07-14 01:06:10</t>
+          <t>2023-07-11</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "169160"| "item__name": "buttermilk yellow digital printed embroidered muslin top with floral print muslin dupatta set"| "visit_count": 1}| {"item__product_id": "176874"| "item__name": "black and beige lace work v neck muslin top with floral muslin dupatta set"| "visit_count": 1}| {"item__product_id": "107117"| "item__name": "bumblebee yellow zari polka weave dola silk top with red banarasi dupatta set"| "visit_count": 1}| {"item__product_id": "175180"| "item__name": "cerulean blue hand embroidered chikankari cotton top with printed cotton dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "161557"| "item__name": "beige and yellow digital printed linen top with chiffon dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "107117"| "item__name": "bumblebee yellow zari polka weave dola silk top with red banarasi dupatta set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Pratima Yadav</t>
+          <t>C. S. Parulekar</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>9226158553</t>
+          <t>7767031974</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2023-07-14 10:44:02</t>
+          <t>2023-07-11</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "145129"| "item__name": "Blue Printed Cotton Top and Bottom with Lace work and Chiffon Dupatta Set"| "visit_count": 3}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"| "visit_count": 3}| {"item__product_id": "176342"| "item__name": "peach floral printed cotton fabric"| "visit_count": 2}| {"item__product_id": "150645"| "item__name": "Mustard Yellow Leheriya Inspired Printed Kota Chikankari Kurti"| "visit_count": 2}| {"item__product_id": "182389"| "item__name": "Zebra Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "170426"| "item__name": "amber yellow cotton dobby top with stripe print dupatta set"| "visit_count": 1}| {"item__product_id": "163597"| "item__name": "Forest Green Tropical Printed Cotton Fabric"| "visit_count": 1}| {"item__product_id": "177150"| "item__name": "purple bandhani inspired printed cotton top"| "visit_count": 1}| {"item__product_id": "175395"| "item__name": "olive green authentic chikankari ikkat top"| "visit_count": 1}| {"item__product_id": "175651"| "item__name": "cosmic yellow hand parsi embroidered chikankari with mukesh work top"| "visit_count": 1}| {"item__product_id": "175180"| "item__name": "cerulean blue hand embroidered chikankari cotton top with printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "138814"| "item__name": "teal green solid kurti with kantha work"| "visit_count": 1}| {"item__product_id": "168423"| "item__name": "spanish orange modal chikankari kurti d2"| "visit_count": 1}| {"item__product_id": "163707"| "item__name": "offwhite khadi cotton trouser"| "visit_count": 1}| {"item__product_id": "167071"| "item__name": "rouge pink dabu work kantha cotton fabric with schiffli"| "visit_count": 1}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"| "visit_count": 1}| {"item__product_id": "165802"| "item__name": "cream cotton schiffli hem fabric"| "visit_count": 1}| {"item__product_id": "177343"| "item__name": "blush pink floral printed cotton chikankari kurti"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "143242"| "item__name": "cadium green printed cotton fabric"| "visit_count": 1}| {"item__product_id": "182439"| "item__name": "Mystic Mauvewood Chanderi Top with Hand Painted Chiffon Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"}| {"item__product_id": "176342"| "item__name": "peach floral printed cotton fabric"}| {"item__product_id": "165802"| "item__name": "cream cotton schiffli hem fabric"}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"}| {"item__product_id": "145129"| "item__name": "Blue Printed Cotton Top and Bottom with Lace work and Chiffon Dupatta Set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>ravi.ranjan</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>6629</t>
-        </is>
-      </c>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Archana sharma</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>9810991771</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2023-07-14 22:28:57</t>
+          <t>2023-07-12</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "162133"| "item__name": "sage green digital printed top with chiffon dupatta set"| "visit_count": 3}| {"item__product_id": "182540"| "item__name": "Barbie Pink Leheriya Printed Lace Work Cotton Top"| "visit_count": 2}| {"item__product_id": "182409"| "item__name": "Laffy Taffy Lavender Embellished Neck Work Organza Top with Organza Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "166662"| "item__name": "dove greyish purple printed chikankari top with leheriya printed palazzo"| "visit_count": 1}| {"item__product_id": "177343"| "item__name": "blush pink floral printed cotton chikankari kurti"| "visit_count": 1}| {"item__product_id": "164902"| "item__name": "goan green tropical printed cotton dress with belt"| "visit_count": 1}| {"item__product_id": "166939"| "item__name": "grape purple plain dress with belt"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "171049"| "item__name": "shades of yellow leheriya printed muslin top with cotton silk dupatta set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Monika Gupta </t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
+          <t>Ruchi Aggarwal</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>9310278584</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2023-07-15 07:12:36</t>
+          <t>2023-07-13</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "178923"| "item__name": "celadon blue thread work cotton top with printed cotton dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "61618"| "item__name": "Red kurti with beige palazzo set"| "visit_count": 1}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1192,55 +1196,55 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Sujata Naresh Behl </t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>9793325176</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>anita.meena</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>6591</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2023-07-15 14:02:39</t>
+          <t>2023-07-13</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182719"| "item__name": "Ghoomer Spruce Blue Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 3}| {"item__product_id": "182722"| "item__name": "Ghoomer Moss Green Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "179954"| "item__name": "cream white cotton top with royal blue chiffon dupatta set"| "visit_count": 3}| {"item__product_id": "154486"| "item__name": "blue ikkat cotton co ord set"| "visit_count": 1}| {"item__product_id": "182438"| "item__name": "Champagne Dream Biege Embellished Neckline Chanderi Top with Leheriya Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182547"| "item__name": "Barbie Blue Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "179931"| "item__name": "cream white cotton top with current red kalamkari dupatta set"| "visit_count": 1}| {"item__product_id": "180004"| "item__name": "cream white cotton top with neon pink patola print dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "179954"| "item__name": "cream white cotton top with royal blue chiffon dupatta set"}]</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>sangeetagandhi74</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>6653</t>
-        </is>
-      </c>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seema sachin punia </t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>9896229484</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2023-07-15 15:41:40</t>
+          <t>2023-07-13</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"| "visit_count": 1}| {"item__product_id": "117527"| "item__name": "crimson pink muslin 3 piece garara set"| "visit_count": 1}| {"item__product_id": "154486"| "item__name": "blue ikkat cotton co ord set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 1}| {"item__product_id": "104294"| "item__name": "black mushru 3 piece set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1250,31 +1254,31 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Pratibha Sharma </t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>8800666288</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Ranjith</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>5749</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2023-07-15 18:47:00</t>
+          <t>2023-07-13</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 2}| {"item__product_id": "173500"| "item__name": "hot pink embellished neck work cotton top with stripe printed chiffon dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "180555"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"| "visit_count": 9}| {"item__product_id": "182290"| "item__name": "Nawabi LiLac Authentic Chikankari Cotton Top with Cotton Dupatta Set"| "visit_count": 7}| {"item__product_id": "164822"| "item__name": "mint green neck thread work kota doriya top and dupatta set"| "visit_count": 6}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"| "visit_count": 6}| {"item__product_id": "182300"| "item__name": "Nawabi Mint Green Authentic Chikankari Cotton Top with Cotton Dupatta Set"| "visit_count": 6}| {"item__product_id": "170419"| "item__name": "hot pink cotton dobby top with stripe print dupatta set"| "visit_count": 5}| {"item__product_id": "170426"| "item__name": "amber yellow cotton dobby top with stripe print dupatta set"| "visit_count": 5}| {"item__product_id": "161155"| "item__name": "flamingo pink kota doriya thread work top with chiffon printed dupatta set"| "visit_count": 5}| {"item__product_id": "182339"| "item__name": "Mohini Light Mauve Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 5}| {"item__product_id": "179506"| "item__name": "Mellow Yellow Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 5}| {"item__product_id": "182749"| "item__name": "Mastani Purple V neck Printed Muslin Top With Thread Work Organza Dupatta Set"| "visit_count": 4}| {"item__product_id": "172384"| "item__name": "maroon red kantha cotton top with rust red ajrak printed dupatta set d2"| "visit_count": 3}| {"item__product_id": "162133"| "item__name": "sage green digital printed top with chiffon dupatta set"| "visit_count": 3}| {"item__product_id": "172385"| "item__name": "mustard yellow kantha cotton top with black ajrak printed dupatta set d2"| "visit_count": 3}| {"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"| "visit_count": 3}| {"item__product_id": "181948"| "item__name": "Eggplant Purple Digital Printed Cotton Linen Top and Dupatta Set-D2"| "visit_count": 3}| {"item__product_id": "179502"| "item__name": "Blush Pink Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 3}| {"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 2}| {"item__product_id": "178784"| "item__name": "mehndi green stripe printed cotton top with floral mul cotton dupatta set"| "visit_count": 2}| {"item__product_id": "182264"| "item__name": "Ribollita Baby Blue Digital Printed Glazed Cotton Top with Organza Dupatta Set"| "visit_count": 2}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 2}| {"item__product_id": "106956"| "item__name": "sky blue floral printed cotton top with stripe bottom and plain chiffon dupatta"| "visit_count": 2}| {"item__product_id": "183087"| "item__name": "Ivory South Cotton V Neck with Mangalgiri Hem with Midnight Blue Dupatta Set"| "visit_count": 2}| {"item__product_id": "173500"| "item__name": "hot pink embellished neck work cotton top with stripe printed chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "177950"| "item__name": "Light Grey Floral Printed Cotton Top With Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}| {"item__product_id": "152076"| "item__name": "Salmon Peach Candy Stripe Printed Cotton Top with Kota Hand Painted Dupatta Set"| "visit_count": 1}| {"item__product_id": "178923"| "item__name": "celadon blue thread work cotton top with printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "131289"| "item__name": "tuscan sun yellow printed cotton top with tie and dye dupatta set"| "visit_count": 1}| {"item__product_id": "176605"| "item__name": "cream white sequin work chanderi top with floral printed chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "181868"| "item__name": "Dark Pink and Magenta South Cotton Top with Mangalgiri Hem and Dupatta Set"| "visit_count": 1}| {"item__product_id": "178922"| "item__name": "opera mauve thread work cotton top with printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "170838"| "item__name": "cyber yellow thread work chanderi top with organza dupatta set"| "visit_count": 1}| {"item__product_id": "182148"| "item__name": "Kesariya Bright Red Georgette Leheriya Top with Leheriya Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "166415"| "item__name": "cream and blue cotton dobby chikankari kurti"| "visit_count": 1}| {"item__product_id": "180386"| "item__name": "Maroon Kalamkari Printed Cotton Top with Dobby Work Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "183016"| "item__name": "Lahori Jade Green Cotton Pakistani Suit with Embroidered Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182355"| "item__name": "Mohini Beige White Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}| {"item__product_id": "177935"| "item__name": "baby pink floral printed cotton top with hand printed kota dupatta set"| "visit_count": 1}| {"item__product_id": "182375"| "item__name": "Leher Violet Purple Cotton Leheriya Top with Shibori Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "177979"| "item__name": "maroon red embellished neck work muslin top with zari work chanderi silk dupatta set"| "visit_count": 1}| {"item__product_id": "173681"| "item__name": "peach embellished neck work zig zag muslin top with plain muslin dupatta set"| "visit_count": 1}| {"item__product_id": "182218"| "item__name": "Savri Lilac Printed Cotton Top with Printed Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "169842"| "item__name": "sapphire blue printed cotton co ord set"| "visit_count": 1}| {"item__product_id": "175082"| "item__name": "light lilac modal chikankari kurti"| "visit_count": 1}| {"item__product_id": "178956"| "item__name": "baby blue stripe jam cotton top with cotton dupatta set"| "visit_count": 1}| {"item__product_id": "169185"| "item__name": "jade green crochet work pakistani suit with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "181470"| "item__name": "Ivory White Plain Lycra Trouser with Lace"| "visit_count": 1}| {"item__product_id": "181604"| "item__name": "Carolina Blue Printed Cotton Top with Cream Bottom and White Printed Kota Dupatta Set"| "visit_count": 1}| {"item__product_id": "148835"| "item__name": "purple and orange printed top and dupatta set"| "visit_count": 1}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"| "visit_count": 1}| {"item__product_id": "180557"| "item__name": "Mulberry Mauve Thread Work Cotton Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "169215"| "item__name": "periwinkle purple floral muslin top with cotton silk dupatta set"| "visit_count": 1}| {"item__product_id": "172734"| "item__name": "lilac printed cotton schiffli kurti"| "visit_count": 1}| {"item__product_id": "176601"| "item__name": "ebony black sequin work chanderi top with floral printed chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "182455"| "item__name": "Space Blue Chanderi Kantha 3 Piece Set"| "visit_count": 1}| {"item__product_id": "176206"| "item__name": "light blue floral printed cotton top with flex cotton co ord set"| "visit_count": 1}| {"item__product_id": "182540"| "item__name": "Barbie Pink Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "166319"| "item__name": "light peach chikankari cotton linen top with schiffli bottom 2 piece set"| "visit_count": 1}| {"item__product_id": "149968"| "item__name": "Pearl White Cotton Schiffli Fabric- 2"| "visit_count": 1}| {"item__product_id": "180004"| "item__name": "cream white cotton top with neon pink patola print dupatta set"| "visit_count": 1}| {"item__product_id": "95820"| "item__name": "offwhite full schiffali work trouser"| "visit_count": 1}| {"item__product_id": "181159"| "item__name": "Denim blue Tussar Chanderi Dupatta"| "visit_count": 1}| {"item__product_id": "182854"| "item__name": "Cobalt Blue South Cotton Top with Mangalgiri Hem and Denim Blue Dupatta Set"| "visit_count": 1}| {"item__product_id": "175054"| "item__name": "blue mix color printed cotton chikankari kurti"| "visit_count": 1}| {"item__product_id": "177437"| "item__name": "black plain cotton flex trouser"| "visit_count": 1}| {"item__product_id": "179507"| "item__name": "Aqua Blue Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "182439"| "item__name": "Mystic Mauvewood Chanderi Top with Hand Painted Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "181955"| "item__name": "Mint Green Digital Printed Cotton Linen Top and Dupatta Set-D2"| "visit_count": 1}| {"item__product_id": "179919"| "item__name": "indigo printed v neck cotton top with printed bottom and dupatta set"| "visit_count": 1}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "168327"| "item__name": "sandcastle beige digital printed floral cotton linen top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "182224"| "item__name": "Mahreen Light Orchid Candy Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "182698"| "item__name": "Nihari Sage Green Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 1}| {"item__product_id": "177946"| "item__name": "midnight black thread work chanderi top with organza dupatta set"| "visit_count": 1}| {"item__product_id": "182401"| "item__name": "Sizzler Baby Pink Authentic Bandhej Top with Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182389"| "item__name": "Zebra Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "116991"| "item__name": "currant red bandhej cotton top with fire yellow dupatta set"| "visit_count": 1}| {"item__product_id": "180249"| "item__name": "Dandelion Yellow Glazed Cotton Printed Top with Glazed Cotton Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "166907"| "item__name": "lapis blue printed cotton top with bumblebee yellow chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "137784"| "item__name": "Fire Red Printed Chikankari Kurti"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "178956"| "item__name": "baby blue stripe jam cotton top with cotton dupatta set"}| {"item__product_id": "182264"| "item__name": "Ribollita Baby Blue Digital Printed Glazed Cotton Top with Organza Dupatta Set"}]</t>
         </is>
       </c>
     </row>
@@ -1283,22 +1287,22 @@
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ankita.singh</t>
+          <t>lil.angl795</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>6659</t>
+          <t>6600</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2023-07-15 19:15:49</t>
+          <t>2023-07-13</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "168546"| "item__name": "lilac muslin 3 piece set with cotton silk dupatta"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1310,58 +1314,58 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mamta Aggarwal </t>
+          <t>Pratima Yadav</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>9818514311</t>
+          <t>9226158553</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2023-07-16 08:37:39</t>
+          <t>2023-07-14</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "176342"| "item__name": "peach floral printed cotton fabric"| "visit_count": 2}| {"item__product_id": "150645"| "item__name": "Mustard Yellow Leheriya Inspired Printed Kota Chikankari Kurti"| "visit_count": 2}| {"item__product_id": "179106"| "item__name": "Sand Beige and Blue Printed Khadi Lace Work Cotton Top"| "visit_count": 2}| {"item__product_id": "145129"| "item__name": "Blue Printed Cotton Top and Bottom with Lace work and Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "177343"| "item__name": "blush pink floral printed cotton chikankari kurti"| "visit_count": 1}| {"item__product_id": "182389"| "item__name": "Zebra Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "163597"| "item__name": "Forest Green Tropical Printed Cotton Fabric"| "visit_count": 1}| {"item__product_id": "177150"| "item__name": "purple bandhani inspired printed cotton top"| "visit_count": 1}| {"item__product_id": "175395"| "item__name": "olive green authentic chikankari ikkat top"| "visit_count": 1}| {"item__product_id": "175651"| "item__name": "cosmic yellow hand parsi embroidered chikankari with mukesh work top"| "visit_count": 1}| {"item__product_id": "175180"| "item__name": "cerulean blue hand embroidered chikankari cotton top with printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "138814"| "item__name": "teal green solid kurti with kantha work"| "visit_count": 1}| {"item__product_id": "168423"| "item__name": "spanish orange modal chikankari kurti d2"| "visit_count": 1}| {"item__product_id": "163707"| "item__name": "offwhite khadi cotton trouser"| "visit_count": 1}| {"item__product_id": "167071"| "item__name": "rouge pink dabu work kantha cotton fabric with schiffli"| "visit_count": 1}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"| "visit_count": 1}| {"item__product_id": "165802"| "item__name": "cream cotton schiffli hem fabric"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "176342"| "item__name": "peach floral printed cotton fabric"}| {"item__product_id": "165802"| "item__name": "cream cotton schiffli hem fabric"}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"}| {"item__product_id": "145129"| "item__name": "Blue Printed Cotton Top and Bottom with Lace work and Chiffon Dupatta Set"}]</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
-      <c r="B32" t="inlineStr"/>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>mrshimanshu1999</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>6670</t>
-        </is>
-      </c>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lalita Saonya </t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>7667275779</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2023-07-16 09:48:24</t>
+          <t>2023-07-14</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"| "visit_count": 1}| {"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "137775"| "item__name": "mint green printed chikankari kurti"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1370,56 +1374,56 @@
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ruchi.mishra</t>
+          <t>ravi.ranjan</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>6689</t>
+          <t>6629</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2023-07-16 16:58:42</t>
+          <t>2023-07-14</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "175651"| "item__name": "cosmic yellow hand parsi embroidered chikankari with mukesh work top"| "visit_count": 1}| {"item__product_id": "179519"| "item__name": "ebony black thread work georgette top with georgette dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "162133"| "item__name": "sage green digital printed top with chiffon dupatta set"| "visit_count": 3}| {"item__product_id": "182540"| "item__name": "Barbie Pink Leheriya Printed Lace Work Cotton Top"| "visit_count": 2}| {"item__product_id": "182409"| "item__name": "Laffy Taffy Lavender Embellished Neck Work Organza Top with Organza Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "171049"| "item__name": "shades of yellow leheriya printed muslin top with cotton silk dupatta set"}]</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr"/>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>richa.arora</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>6692</t>
-        </is>
-      </c>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sujata Naresh Behl </t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>9793325176</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2023-07-16 21:32:53</t>
+          <t>2023-07-15</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "178640"| "item__name": "Creamy White Printed Cotton Top and Teal Green Bottom with Cotton Dupatta Set"| "visit_count": 2}| {"item__product_id": "142912"| "item__name": "mauve kantha printed 2 piece set"| "visit_count": 2}| {"item__product_id": "160036"| "item__name": "pistachio green print on print 2 piece set"| "visit_count": 2}| {"item__product_id": "109151"| "item__name": "white applique scallop palazzo trouser"| "visit_count": 1}| {"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "176874"| "item__name": "black and beige lace work v neck muslin top with floral muslin dupatta set"| "visit_count": 1}| {"item__product_id": "182547"| "item__name": "Barbie Blue Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "162669"| "item__name": "blond yellow printed cotton top with grey printed dupatta set"| "visit_count": 1}| {"item__product_id": "179931"| "item__name": "cream white cotton top with current red kalamkari dupatta set"| "visit_count": 1}| {"item__product_id": "167120"| "item__name": "carrot peach kota all over thread work top with kota dupatta 3 piece set"| "visit_count": 1}| {"item__product_id": "112196"| "item__name": "corn yellow satin silk 3 piece set with organza dupatta"| "visit_count": 1}| {"item__product_id": "171011"| "item__name": "daisy white thread work 3 piece set with chiffon dupatta"| "visit_count": 1}| {"item__product_id": "179214"| "item__name": "indigo dabu work kantha cotton kurti"| "visit_count": 1}| {"item__product_id": "148501"| "item__name": "off white printed cotton linen with chiffon dupatta 3 piece set"| "visit_count": 1}| {"item__product_id": "161274"| "item__name": "sapphire blue stripe printed cotton top with kota hand painted dupatta 3 piece set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182719"| "item__name": "Ghoomer Spruce Blue Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 3}| {"item__product_id": "182722"| "item__name": "Ghoomer Moss Green Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "162669"| "item__name": "blond yellow printed cotton top with grey printed dupatta set"}| {"item__product_id": "178640"| "item__name": "Creamy White Printed Cotton Top and Teal Green Bottom with Cotton Dupatta Set"}| {"item__product_id": "179214"| "item__name": "indigo dabu work kantha cotton kurti"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1428,22 +1432,22 @@
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>manish.kumar</t>
+          <t>sangeetagandhi74</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>6696</t>
+          <t>6653</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2023-07-16 23:42:59</t>
+          <t>2023-07-15</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182856"| "item__name": "Faded Brown South Cotton Top with Mangalgiri Hem with Dark Barn Red Dupatta"| "visit_count": 3}| {"item__product_id": "163645"| "item__name": "mulberry green abstract printed cotton fabric"| "visit_count": 1}| {"item__product_id": "179507"| "item__name": "Aqua Blue Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "176234"| "item__name": "light beige chanderi top with zig zag printed chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"| "visit_count": 1}| {"item__product_id": "178608"| "item__name": "Iris Purple Digital Printed Muslin Top with Printed Chanderi Silk Dupatta set"| "visit_count": 1}| {"item__product_id": "130755"| "item__name": "moss green printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 1}| {"item__product_id": "159102"| "item__name": "Raisin and Cream Printed Cotton Top with Cream Chiffon Hand Painted Dupatta Set"| "visit_count": 1}| {"item__product_id": "182224"| "item__name": "Mahreen Light Orchid Candy Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}| {"item__product_id": "177935"| "item__name": "baby pink floral printed cotton top with hand printed kota dupatta set"| "visit_count": 1}| {"item__product_id": "182857"| "item__name": "Light Grey Printed South Cotton Top with Mangalgiri Hem With Black Dupatta Set"| "visit_count": 1}| {"item__product_id": "159525"| "item__name": "light orange south cotton top with mangalgiri hem with barn red dupatta"| "visit_count": 1}| {"item__product_id": "181029"| "item__name": "Cerulean Blue Flower Printed Cotton fabric"| "visit_count": 1}| {"item__product_id": "144772"| "item__name": "navy blue printed cotton fabric 3 with maroon flax cotton fabric"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "117527"| "item__name": "crimson pink muslin 3 piece garara set"| "visit_count": 1}| {"item__product_id": "154486"| "item__name": "blue ikkat cotton co ord set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1455,24 +1459,24 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Deepali kachhap</t>
+          <t xml:space="preserve">Pratibha Sharma </t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>9570182557</t>
+          <t>8800666288</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2023-07-17 09:59:45</t>
+          <t>2023-07-15</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "179908"| "item__name": "cinnamon brown cotton linen floral chikankari work kurti"| "visit_count": 1}| {"item__product_id": "151404"| "item__name": "grey and purple zig zig printed chikankari kurti"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 2}| {"item__product_id": "173500"| "item__name": "hot pink embellished neck work cotton top with stripe printed chiffon dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1484,24 +1488,24 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shruti </t>
+          <t xml:space="preserve">Mamta Aggarwal </t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7607540210</t>
+          <t>9818514311</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2023-07-17 16:26:10</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "179507"| "item__name": "Aqua Blue Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 2}| {"item__product_id": "170426"| "item__name": "amber yellow cotton dobby top with stripe print dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1515,56 +1519,56 @@
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>neeraj.bala</t>
+          <t>mrshimanshu1999</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>6710</t>
+          <t>6670</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2023-07-17 16:29:40</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "173489"| "item__name": "royal blue floral digital gather work printed chanderi top with chanderi top"| "visit_count": 1}| {"item__product_id": "171030"| "item__name": "carolina blue dola silk top with embellished neck line and banarasi dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"| "visit_count": 1}| {"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"}| {"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"}]</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Vandana sharma</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>8800241877</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>richa.arora</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>6692</t>
+        </is>
+      </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2023-07-18 02:58:09</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "109151"| "item__name": "white applique scallop palazzo trouser"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "178640"| "item__name": "Creamy White Printed Cotton Top and Teal Green Bottom with Cotton Dupatta Set"| "visit_count": 2}| {"item__product_id": "142912"| "item__name": "mauve kantha printed 2 piece set"| "visit_count": 2}| {"item__product_id": "160036"| "item__name": "pistachio green print on print 2 piece set"| "visit_count": 2}| {"item__product_id": "109151"| "item__name": "white applique scallop palazzo trouser"| "visit_count": 1}| {"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "176874"| "item__name": "black and beige lace work v neck muslin top with floral muslin dupatta set"| "visit_count": 1}| {"item__product_id": "182547"| "item__name": "Barbie Blue Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "162669"| "item__name": "blond yellow printed cotton top with grey printed dupatta set"| "visit_count": 1}| {"item__product_id": "179931"| "item__name": "cream white cotton top with current red kalamkari dupatta set"| "visit_count": 1}| {"item__product_id": "167120"| "item__name": "carrot peach kota all over thread work top with kota dupatta 3 piece set"| "visit_count": 1}| {"item__product_id": "112196"| "item__name": "corn yellow satin silk 3 piece set with organza dupatta"| "visit_count": 1}| {"item__product_id": "171011"| "item__name": "daisy white thread work 3 piece set with chiffon dupatta"| "visit_count": 1}| {"item__product_id": "179214"| "item__name": "indigo dabu work kantha cotton kurti"| "visit_count": 1}| {"item__product_id": "148501"| "item__name": "off white printed cotton linen with chiffon dupatta 3 piece set"| "visit_count": 1}| {"item__product_id": "161274"| "item__name": "sapphire blue stripe printed cotton top with kota hand painted dupatta 3 piece set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "162669"| "item__name": "blond yellow printed cotton top with grey printed dupatta set"}| {"item__product_id": "178640"| "item__name": "Creamy White Printed Cotton Top and Teal Green Bottom with Cotton Dupatta Set"}| {"item__product_id": "179214"| "item__name": "indigo dabu work kantha cotton kurti"}]</t>
         </is>
       </c>
     </row>
@@ -1573,109 +1577,109 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>sweta.archana</t>
+          <t>manish.kumar</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>6720</t>
+          <t>6696</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2023-07-18 10:44:25</t>
+          <t>2023-07-16</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 3}| {"item__product_id": "180391"| "item__name": "Egyptian Teal Applique Work Glazed Cotton Top with Art Chanderi Dupatta Set"| "visit_count": 3}| {"item__product_id": "181842"| "item__name": "Orange South Cotton Top with Mangalgiri Hem with Red Dupatta Set"| "visit_count": 3}| {"item__product_id": "182955"| "item__name": "Afreen Beige French Knot Cotton Top with French Knot Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "169278"| "item__name": "ruby red embellished work georgette top with embroidered georgette dupatta set"| "visit_count": 1}| {"item__product_id": "182037"| "item__name": "Ruhani Red Dark Green Ajrak Printed Cotton Top With Block Printed Kota Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182856"| "item__name": "Faded Brown South Cotton Top with Mangalgiri Hem with Dark Barn Red Dupatta"| "visit_count": 3}| {"item__product_id": "163645"| "item__name": "mulberry green abstract printed cotton fabric"| "visit_count": 1}| {"item__product_id": "179507"| "item__name": "Aqua Blue Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "176234"| "item__name": "light beige chanderi top with zig zag printed chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"| "visit_count": 1}| {"item__product_id": "178608"| "item__name": "Iris Purple Digital Printed Muslin Top with Printed Chanderi Silk Dupatta set"| "visit_count": 1}| {"item__product_id": "130755"| "item__name": "moss green printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 1}| {"item__product_id": "159102"| "item__name": "Raisin and Cream Printed Cotton Top with Cream Chiffon Hand Painted Dupatta Set"| "visit_count": 1}| {"item__product_id": "182224"| "item__name": "Mahreen Light Orchid Candy Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}| {"item__product_id": "177935"| "item__name": "baby pink floral printed cotton top with hand printed kota dupatta set"| "visit_count": 1}| {"item__product_id": "182857"| "item__name": "Light Grey Printed South Cotton Top with Mangalgiri Hem With Black Dupatta Set"| "visit_count": 1}| {"item__product_id": "159525"| "item__name": "light orange south cotton top with mangalgiri hem with barn red dupatta"| "visit_count": 1}| {"item__product_id": "181029"| "item__name": "Cerulean Blue Flower Printed Cotton fabric"| "visit_count": 1}| {"item__product_id": "144772"| "item__name": "navy blue printed cotton fabric 3 with maroon flax cotton fabric"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "180391"| "item__name": "Egyptian Teal Applique Work Glazed Cotton Top with Art Chanderi Dupatta Set"}| {"item__product_id": "180391"| "item__name": "Egyptian Teal Applique Work Glazed Cotton Top with Art Chanderi Dupatta Set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "181842"| "item__name": "Orange South Cotton Top with Mangalgiri Hem with Red Dupatta Set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Reshma S</t>
+          <t>Deepali kachhap</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8897611007</t>
+          <t>9570182557</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2023-07-18 10:49:30</t>
+          <t>2023-07-17</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 2}| {"item__product_id": "182857"| "item__name": "Light Grey Printed South Cotton Top with Mangalgiri Hem With Black Dupatta Set"| "visit_count": 2}| {"item__product_id": "159102"| "item__name": "Raisin and Cream Printed Cotton Top with Cream Chiffon Hand Painted Dupatta Set"| "visit_count": 1}| {"item__product_id": "172432"| "item__name": "creamy white embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "172433"| "item__name": "hazel wood beige embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "178970"| "item__name": "powder beige embellished neck work cotton chanderi top with sapphire blue chanderi silk dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "179908"| "item__name": "cinnamon brown cotton linen floral chikankari work kurti"| "visit_count": 1}| {"item__product_id": "151404"| "item__name": "grey and purple zig zig printed chikankari kurti"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>winrsin2003</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>6721</t>
-        </is>
-      </c>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shruti </t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>7607540210</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2023-07-18 10:52:25</t>
+          <t>2023-07-17</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 2}| {"item__product_id": "182857"| "item__name": "Light Grey Printed South Cotton Top with Mangalgiri Hem With Black Dupatta Set"| "visit_count": 2}| {"item__product_id": "159102"| "item__name": "Raisin and Cream Printed Cotton Top with Cream Chiffon Hand Painted Dupatta Set"| "visit_count": 1}| {"item__product_id": "172432"| "item__name": "creamy white embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "172433"| "item__name": "hazel wood beige embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "178970"| "item__name": "powder beige embellished neck work cotton chanderi top with sapphire blue chanderi silk dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "179507"| "item__name": "Aqua Blue Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>neha</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>9622284104</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>neeraj.bala</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>6710</t>
+        </is>
+      </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2023-07-18 16:11:11</t>
+          <t>2023-07-17</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "178604"| "item__name": "fossil grey chanderi top and floral printed organza dupatta set"| "visit_count": 1}| {"item__product_id": "173836"| "item__name": "slime green v neck muslin top with muslin dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "173489"| "item__name": "royal blue floral digital gather work printed chanderi top with chanderi top"| "visit_count": 1}| {"item__product_id": "171030"| "item__name": "carolina blue dola silk top with embellished neck line and banarasi dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -1689,192 +1693,192 @@
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>mahua.majumder</t>
+          <t>sweta.archana</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>6732</t>
+          <t>6720</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2023-07-18 17:12:41</t>
+          <t>2023-07-18</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}| {"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "181842"| "item__name": "Orange South Cotton Top with Mangalgiri Hem with Red Dupatta Set"| "visit_count": 3}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "180391"| "item__name": "Egyptian Teal Applique Work Glazed Cotton Top with Art Chanderi Dupatta Set"| "visit_count": 1}| {"item__product_id": "182955"| "item__name": "Afreen Beige French Knot Cotton Top with French Knot Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "169278"| "item__name": "ruby red embellished work georgette top with embroidered georgette dupatta set"| "visit_count": 1}| {"item__product_id": "182037"| "item__name": "Ruhani Red Dark Green Ajrak Printed Cotton Top With Block Printed Kota Dupatta Set"| "visit_count": 1}| {"item__product_id": "177963"| "item__name": "bright pink georgette leheriya top with leheriya chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "171030"| "item__name": "carolina blue dola silk top with embellished neck line and banarasi dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}]</t>
+          <t>[{"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"}| {"item__product_id": "181842"| "item__name": "Orange South Cotton Top with Mangalgiri Hem with Red Dupatta Set"}]</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Triveni Shekar </t>
+          <t>Reshma S</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>09986357770</t>
+          <t>8897611007</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2023-07-19 10:18:39</t>
+          <t>2023-07-18</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 2}| {"item__product_id": "180339"| "item__name": "black ajrak patch jam satin top with offwhite printed dupatta set d2"| "visit_count": 2}| {"item__product_id": "176297"| "item__name": "tortilla beige v neck cotton flax top"| "visit_count": 2}| {"item__product_id": "130755"| "item__name": "moss green printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 2}| {"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "159521"| "item__name": "grey south cotton temple hem with dark denim blue dupatta set"| "visit_count": 2}| {"item__product_id": "176359"| "item__name": "pearl white french knot cotton top with purple authentic french knot dupatta set d2"| "visit_count": 2}| {"item__product_id": "159525"| "item__name": "light orange south cotton top with mangalgiri hem with barn red dupatta"| "visit_count": 1}| {"item__product_id": "172734"| "item__name": "lilac printed cotton schiffli kurti"| "visit_count": 1}| {"item__product_id": "176269"| "item__name": "creamy pink floral printed cotton top"| "visit_count": 1}| {"item__product_id": "162133"| "item__name": "sage green digital printed top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "182264"| "item__name": "Ribollita Baby Blue Digital Printed Glazed Cotton Top with Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "182408"| "item__name": "Sizzler Bright Yellow Authentic Bandhej Top with Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "176364"| "item__name": "teal blue authentic bandhej top with cotton dupatta set d2"| "visit_count": 1}| {"item__product_id": "182547"| "item__name": "Barbie Blue Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "182224"| "item__name": "Mahreen Light Orchid Candy Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "170806"| "item__name": "persian pink digital printed cotton top with tie dye chiffon dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 2}| {"item__product_id": "182857"| "item__name": "Light Grey Printed South Cotton Top with Mangalgiri Hem With Black Dupatta Set"| "visit_count": 2}| {"item__product_id": "159102"| "item__name": "Raisin and Cream Printed Cotton Top with Cream Chiffon Hand Painted Dupatta Set"| "visit_count": 1}| {"item__product_id": "172432"| "item__name": "creamy white embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "172433"| "item__name": "hazel wood beige embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "178970"| "item__name": "powder beige embellished neck work cotton chanderi top with sapphire blue chanderi silk dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "180339"| "item__name": "black ajrak patch jam satin top with offwhite printed dupatta set d2"}| {"item__product_id": "176297"| "item__name": "tortilla beige v neck cotton flax top"}| {"item__product_id": "130755"| "item__name": "moss green printed chanderi top with kantha inspired printed dupatta set"}| {"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"}| {"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"}| {"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"}| {"item__product_id": "176364"| "item__name": "teal blue authentic bandhej top with cotton dupatta set d2"}| {"item__product_id": "176269"| "item__name": "creamy pink floral printed cotton top"}| {"item__product_id": "176359"| "item__name": "pearl white french knot cotton top with purple authentic french knot dupatta set d2"}]</t>
+          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"}]</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>winrsin2003</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>6721</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2023-07-18</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 2}| {"item__product_id": "182857"| "item__name": "Light Grey Printed South Cotton Top with Mangalgiri Hem With Black Dupatta Set"| "visit_count": 2}| {"item__product_id": "159102"| "item__name": "Raisin and Cream Printed Cotton Top with Cream Chiffon Hand Painted Dupatta Set"| "visit_count": 1}| {"item__product_id": "172432"| "item__name": "creamy white embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "172433"| "item__name": "hazel wood beige embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "178970"| "item__name": "powder beige embellished neck work cotton chanderi top with sapphire blue chanderi silk dupatta set"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Triveni Shekar </t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>09986357770</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2023-07-19</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "176359"| "item__name": "pearl white french knot cotton top with purple authentic french knot dupatta set d2"| "visit_count": 2}| {"item__product_id": "159521"| "item__name": "grey south cotton temple hem with dark denim blue dupatta set"| "visit_count": 2}| {"item__product_id": "170806"| "item__name": "persian pink digital printed cotton top with tie dye chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "182224"| "item__name": "Mahreen Light Orchid Candy Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "182547"| "item__name": "Barbie Blue Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "176364"| "item__name": "teal blue authentic bandhej top with cotton dupatta set d2"| "visit_count": 1}| {"item__product_id": "182408"| "item__name": "Sizzler Bright Yellow Authentic Bandhej Top with Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "182264"| "item__name": "Ribollita Baby Blue Digital Printed Glazed Cotton Top with Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "162133"| "item__name": "sage green digital printed top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "176269"| "item__name": "creamy pink floral printed cotton top"| "visit_count": 1}| {"item__product_id": "159525"| "item__name": "light orange south cotton top with mangalgiri hem with barn red dupatta"| "visit_count": 1}| {"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "180339"| "item__name": "black ajrak patch jam satin top with offwhite printed dupatta set d2"| "visit_count": 1}| {"item__product_id": "130755"| "item__name": "moss green printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 1}| {"item__product_id": "176297"| "item__name": "tortilla beige v neck cotton flax top"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"}| {"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"}| {"item__product_id": "176364"| "item__name": "teal blue authentic bandhej top with cotton dupatta set d2"}| {"item__product_id": "176269"| "item__name": "creamy pink floral printed cotton top"}| {"item__product_id": "176359"| "item__name": "pearl white french knot cotton top with purple authentic french knot dupatta set d2"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
         <is>
           <t>Sumitha Indra Kumar</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>9845605562</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>2023-07-19 11:23:59</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>[{"item__product_id": "179104"| "item__name": "Sapphire Blue Floral Printed Cotton Top"| "visit_count": 1}| {"item__product_id": "182857"| "item__name": "Light Grey Printed South Cotton Top with Mangalgiri Hem With Black Dupatta Set"| "visit_count": 1}| {"item__product_id": "167074"| "item__name": "indigo dabu work kantha cotton fabric with schiffali fabric"| "visit_count": 1}| {"item__product_id": "179214"| "item__name": "indigo dabu work kantha cotton kurti"| "visit_count": 1}| {"item__product_id": "143638"| "item__name": "yellow block printed cotton fabric"| "visit_count": 1}]</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr"/>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr">
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2023-07-19</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "179214"| "item__name": "indigo dabu work kantha cotton kurti"| "visit_count": 2}| {"item__product_id": "179104"| "item__name": "Sapphire Blue Floral Printed Cotton Top"| "visit_count": 1}| {"item__product_id": "182857"| "item__name": "Light Grey Printed South Cotton Top with Mangalgiri Hem With Black Dupatta Set"| "visit_count": 1}| {"item__product_id": "167074"| "item__name": "indigo dabu work kantha cotton fabric with schiffali fabric"| "visit_count": 1}| {"item__product_id": "143638"| "item__name": "yellow block printed cotton fabric"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr">
         <is>
           <t>durga.gulmohar</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>6745</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>2023-07-19 14:19:33</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2023-07-19</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
         <is>
           <t>[{"item__product_id": "161557"| "item__name": "beige and yellow digital printed linen top with chiffon dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr"/>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>shailjamakhija</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>6757</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>2023-07-20 10:18:22</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>[{"item__product_id": "180339"| "item__name": "black ajrak patch jam satin top with offwhite printed dupatta set d2"| "visit_count": 2}| {"item__product_id": "179507"| "item__name": "Aqua Blue Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "182547"| "item__name": "Barbie Blue Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "138758"| "item__name": "charcoal grey self digital printed top and dupatta set 2"| "visit_count": 1}]</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>Asha 9517730869</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>2023-07-20 16:24:52</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>[{"item__product_id": "181886"| "item__name": "Eggplant Purple Authentic Bandhej Top with Cotton Dupatta Set"| "visit_count": 1}]</t>
-        </is>
-      </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "181886"| "item__name": "Eggplant Purple Authentic Bandhej Top with Cotton Dupatta Set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Anil sood </t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>7973502614</t>
-        </is>
-      </c>
+          <t>Daksha solanki Makwana</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2023-07-20 22:22:22</t>
+          <t>2023-07-19</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "128988"| "item__name": "mellow yellow printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "153649"| "item__name": "purple with orange highlights cotton 3 piece set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -1884,55 +1888,55 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Iti sharma</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>8433441195</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>raj kiran.solanki</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>6748</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2023-07-21 16:30:15</t>
+          <t>2023-07-19</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "183017"| "item__name": "Lahori Pink Cotton Pakistani Suits with Digital Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182962"| "item__name": "Barbie World Pink French Knot Cotton Top with Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182749"| "item__name": "Mastani Purple V neck Printed Muslin Top With Thread Work Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "182438"| "item__name": "Champagne Dream Biege Embellished Neckline Chanderi Top with Leheriya Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "180386"| "item__name": "Maroon Kalamkari Printed Cotton Top with Dobby Work Chiffon Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "96007"| "item__name": "black straight fit kurti"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Ambika hans</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>9501566806</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>shailjamakhija</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>6757</t>
+        </is>
+      </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2023-07-21 17:01:41</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "180004"| "item__name": "cream white cotton top with neon pink patola print dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "180339"| "item__name": "black ajrak patch jam satin top with offwhite printed dupatta set d2"| "visit_count": 2}| {"item__product_id": "138758"| "item__name": "charcoal grey self digital printed top and dupatta set 2"| "visit_count": 2}| {"item__product_id": "179507"| "item__name": "Aqua Blue Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "182547"| "item__name": "Barbie Blue Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -1944,24 +1948,24 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Anupama sukhavasi</t>
+          <t>Nidhi  Aggarwal</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>8106988979</t>
+          <t>8699415369</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2023-07-21 19:31:27</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182079"| "item__name": "Pardesiya Mint Green Thread Work Chanderi Top with Thread Work Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "61172"| "item__name": "8 baby pink bandhani printed kurti"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "183087"| "item__name": "Ivory South Cotton V Neck with Mangalgiri Hem with Midnight Blue Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -1971,113 +1975,109 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr"/>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Asha 9517730869</t>
+        </is>
+      </c>
       <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>karishma.thadani</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>6780</t>
-        </is>
-      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2023-07-21 19:39:44</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"| "visit_count": 1}| {"item__product_id": "182300"| "item__name": "Nawabi Mint Green Authentic Chikankari Cotton Top with Cotton Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "181886"| "item__name": "Eggplant Purple Authentic Bandhej Top with Cotton Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "181886"| "item__name": "Eggplant Purple Authentic Bandhej Top with Cotton Dupatta Set"}]</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr"/>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>srujanamarella13</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>6789</t>
-        </is>
-      </c>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anil sood </t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>7973502614</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2023-07-22 11:06:21</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182699"| "item__name": "Nihari Bluish Grey Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "128988"| "item__name": "mellow yellow printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182455"| "item__name": "Space Blue Chanderi Kantha 3 Piece Set"}| {"item__product_id": "182699"| "item__name": "Nihari Bluish Grey Chanderi Silk Top with Printed Organza  Dupatta Set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Baljinder Kaur</t>
+          <t xml:space="preserve">Shabana khatoon </t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7780866002</t>
+          <t>8954006747</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2023-07-22 13:10:07</t>
+          <t>2023-07-21</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182857"| "item__name": "Light Grey Printed South Cotton Top with Mangalgiri Hem With Black Dupatta Set"| "visit_count": 6}| {"item__product_id": "182156"| "item__name": "Blissta Black Embellished Neck Work Silk Top With Banarasi Dupatta Set"| "visit_count": 1}| {"item__product_id": "176874"| "item__name": "black and beige lace work v neck muslin top with floral muslin dupatta set"| "visit_count": 1}| {"item__product_id": "173694"| "item__name": "black printed v neck cotton top with semi georgette and cotton dupatta set d2"| "visit_count": 1}| {"item__product_id": "181639"| "item__name": "Ebony Black Katan Staple Handloom Top and Dupatta Set"| "visit_count": 1}| {"item__product_id": "176601"| "item__name": "ebony black sequin work chanderi top with floral printed chanderi dupatta set"| "visit_count": 1}| {"item__product_id": "177946"| "item__name": "midnight black thread work chanderi top with organza dupatta set"| "visit_count": 1}| {"item__product_id": "150958"| "item__name": "barley cream organza thread work top with colorful chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "182195"| "item__name": "Lehar Salmon Peach Lace Work Leheriya Cotton Top With Semi Cotton and Organza Dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "183051"| "item__name": "Rushna Mauve Pink Cotton Silk Top with Thread Work Organza Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "173694"| "item__name": "black printed v neck cotton top with semi georgette and cotton dupatta set d2"}| {"item__product_id": "173694"| "item__name": "black printed v neck cotton top with semi georgette and cotton dupatta set d2"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vandana dobhal </t>
+          <t>Sarita Phogat</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8077761178</t>
+          <t>7015172221</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2023-07-22 22:20:39</t>
+          <t>2023-07-21</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "126319"| "item__name": "almond stripe printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182409"| "item__name": "Laffy Taffy Lavender Embellished Neck Work Organza Top with Organza Printed Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -2089,24 +2089,24 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Mrs Lamba</t>
+          <t xml:space="preserve">Nayeema Rahaman </t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>9899207911</t>
+          <t>9830364319</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2023-07-23 02:22:09</t>
+          <t>2023-07-21</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182224"| "item__name": "Mahreen Light Orchid Candy Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "183075"| "item__name": "Ada Base Grey with Cerulean Blue Floral Cotton Silk Top with Thread Work Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "183077"| "item__name": "Mughal White with Lavender Printed Angrakha Cotton Top with Dual Shade Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182955"| "item__name": "Afreen Beige French Knot Cotton Top with French Knot Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "183004"| "item__name": "Lahori Maroon Cotton Pakistani Suit with Embroidered Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 1}| {"item__product_id": "161557"| "item__name": "beige and yellow digital printed linen top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -2118,24 +2118,24 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Mridula jha</t>
+          <t>Chetna Rohit dave</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>9886043843</t>
+          <t>9925005926</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2023-07-23 11:26:21</t>
+          <t>2023-07-22</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "179529"| "item__name": "Light Blue Floral Embroidered Neck Work with Sequence Work Chiffon Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -2145,142 +2145,142 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Rashmi Bangia </t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>9717525559</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>srujanamarella13</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>6789</t>
+        </is>
+      </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2023-07-23 11:30:13</t>
+          <t>2023-07-22</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "170097"| "item__name": "sepia brown and white printed cotton top with stripe printed dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182699"| "item__name": "Nihari Bluish Grey Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 1}| {"item__product_id": "182731"| "item__name": "Ruhi Mauve Pink Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182955"| "item__name": "Afreen Beige French Knot Cotton Top with French Knot Cotton Dupatta Set"| "visit_count": 1}| {"item__product_id": "182892"| "item__name": "Coca Cola Black Kantha Work Cotton Top with Chanderi Dupatta Set"| "visit_count": 1}| {"item__product_id": "181955"| "item__name": "Mint Green Digital Printed Cotton Linen Top and Dupatta Set-D2"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "182455"| "item__name": "Space Blue Chanderi Kantha 3 Piece Set"}| {"item__product_id": "182699"| "item__name": "Nihari Bluish Grey Chanderi Silk Top with Printed Organza  Dupatta Set"}| {"item__product_id": "181955"| "item__name": "Mint Green Digital Printed Cotton Linen Top and Dupatta Set-D2"}]</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>Yasmin Shaikh</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>9370490043</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>alkesh.tomar</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>6791</t>
+        </is>
+      </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2023-07-23 12:54:36</t>
+          <t>2023-07-22</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "130943"| "item__name": "Raisin Purple Velvet Top and Brocade Bottom Set"| "visit_count": 4}| {"item__product_id": "148544"| "item__name": "ivory georgette chikankari work 3 piece set with chiffon dupatta"| "visit_count": 3}| {"item__product_id": "164768"| "item__name": "ivory south cotton with mangalgiri hem with midnight blue dupatta set"| "visit_count": 2}| {"item__product_id": "179502"| "item__name": "Blush Pink Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "178613"| "item__name": "baby pink thread work georgette top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "180386"| "item__name": "Maroon Kalamkari Printed Cotton Top with Dobby Work Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182833"| "item__name": "Ruhi Purple Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "177177"| "item__name": "baby blue chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "115461"| "item__name": "Basil Green South Cotton Top with Mangalgiri Hem with Barn Red Dupatta"| "visit_count": 1}| {"item__product_id": "182962"| "item__name": "Barbie World Pink French Knot Cotton Top with Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182540"| "item__name": "Barbie Pink Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "169710"| "item__name": "burgundy digital printed top with kantha dupatta set"| "visit_count": 1}| {"item__product_id": "182730"| "item__name": "Ruhi Rust Orange Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182389"| "item__name": "Zebra Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}| {"item__product_id": "177019"| "item__name": "blue and white floral chikankari kurti"| "visit_count": 1}| {"item__product_id": "182339"| "item__name": "Mohini Light Mauve Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}| {"item__product_id": "171768"| "item__name": "black floral designer neck work muslin top with organza dupatta set"| "visit_count": 1}| {"item__product_id": "173694"| "item__name": "black printed v neck cotton top with semi georgette and cotton dupatta set d2"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182962"| "item__name": "Barbie World Pink French Knot Cotton Top with Chiffon Dupatta Set"}| {"item__product_id": "159525"| "item__name": "light orange south cotton top with mangalgiri hem with barn red dupatta"}| {"item__product_id": "181993"| "item__name": "White Cotton Cross Stitch Work Top with White Dupatta Set-1.0"}| {"item__product_id": "148544"| "item__name": "ivory georgette chikankari work 3 piece set with chiffon dupatta"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aaryaa H Bhavsar </t>
+          <t>Baljinder Kaur</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8200794272</t>
+          <t>7780866002</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2023-07-23 14:54:13</t>
+          <t>2023-07-22</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "178613"| "item__name": "baby pink thread work georgette top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "150958"| "item__name": "barley cream organza thread work top with colorful chiffon dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "137057"| "item__name": "light orchid candy stripe printed cotton top with kota hand painted dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "179514"| "item__name": "beige embellished neckline chanderi top with floral printed organza dupatta set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Atish Kamble</t>
+          <t xml:space="preserve">Vandana dobhal </t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>9370706662</t>
+          <t>8077761178</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2023-07-23 14:55:02</t>
+          <t>2023-07-22</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "130320"| "item__name": "magenta south cotton top with mangalgiri hem with parrot green dupatta"| "visit_count": 5}]</t>
+          <t>[{"item__product_id": "126319"| "item__name": "almond stripe printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "130320"| "item__name": "magenta south cotton top with mangalgiri hem with parrot green dupatta"}| {"item__product_id": "130320"| "item__name": "magenta south cotton top with mangalgiri hem with parrot green dupatta"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Priya Shah</t>
+          <t>Mrs Lamba</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>9067450122</t>
+          <t>9899207911</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2023-07-23 15:11:49</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"| "visit_count": 1}| {"item__product_id": "179176"| "item__name": "sage green schiffli cotton dobby short dress"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182224"| "item__name": "Mahreen Light Orchid Candy Stripe Printed Cotton Linen Top with Cotton Linen Printed Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -2290,55 +2290,55 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr"/>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>neha.narang</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>6807</t>
-        </is>
-      </c>
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Monicka</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>7011375215</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2023-07-23 16:21:33</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 2}| {"item__product_id": "143701"| "item__name": "Black Printed Cotton Fabric- 1"| "visit_count": 2}| {"item__product_id": "180838"| "item__name": "Grey Floral Printed Cotton Top Fabric"| "visit_count": 1}| {"item__product_id": "138814"| "item__name": "teal green solid kurti with kantha work"| "visit_count": 1}| {"item__product_id": "152231"| "item__name": "navy blue straight fit kurti"| "visit_count": 1}| {"item__product_id": "97351"| "item__name": "maroon straight fit kurti"| "visit_count": 1}| {"item__product_id": "153375"| "item__name": "brownish grey printed georgette chikankari kurti"| "visit_count": 1}| {"item__product_id": "160036"| "item__name": "pistachio green print on print 2 piece set"| "visit_count": 1}| {"item__product_id": "61618"| "item__name": "Red kurti with beige palazzo set"| "visit_count": 1}| {"item__product_id": "136467"| "item__name": "Mustard Yellow Kantha Cotton Top with Rust Red Ajrak Printed Dupatta 3 Piece Set"| "visit_count": 1}| {"item__product_id": "117097"| "item__name": "mahogany chanderi kantha 3 piece set"| "visit_count": 1}| {"item__product_id": "138018"| "item__name": "maroon kantha cotton top with black ajrak printed dupatta 3 piece set"| "visit_count": 1}| {"item__product_id": "182731"| "item__name": "Ruhi Mauve Pink Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182038"| "item__name": "Ruhani Midnight Blue Ajrak Printed Cotton Top With Block Printed Kota Dupatta Set"| "visit_count": 1}| {"item__product_id": "182856"| "item__name": "Faded Brown South Cotton Top with Mangalgiri Hem with Dark Barn Red Dupatta"| "visit_count": 1}| {"item__product_id": "162750"| "item__name": "flamingo pink printed chikankari kurti"| "visit_count": 1}| {"item__product_id": "166895"| "item__name": "blue and beige stripe co ord set"| "visit_count": 1}| {"item__product_id": "143702"| "item__name": "Black Printed Cotton Fabric- 2"| "visit_count": 1}| {"item__product_id": "181670"| "item__name": "Blue and Pink Printed Cotton Fabric"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "143701"| "item__name": "Black Printed Cotton Fabric- 1"}| {"item__product_id": "143701"| "item__name": "Black Printed Cotton Fabric- 1"}| {"item__product_id": "143702"| "item__name": "Black Printed Cotton Fabric- 2"}| {"item__product_id": "143702"| "item__name": "Black Printed Cotton Fabric- 2"}| {"item__product_id": "97351"| "item__name": "maroon straight fit kurti"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Babloo Ahmad</t>
+          <t>Mridula jha</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>9113755071</t>
+          <t>9886043843</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2023-07-23 16:26:32</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "180339"| "item__name": "black ajrak patch jam satin top with offwhite printed dupatta set d2"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "179529"| "item__name": "Light Blue Floral Embroidered Neck Work with Sequence Work Chiffon Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -2350,24 +2350,24 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shweta undre </t>
+          <t xml:space="preserve">Rashmi Bangia </t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>9922432404</t>
+          <t>9717525559</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2023-07-23 16:46:22</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "166662"| "item__name": "dove greyish purple printed chikankari top with leheriya printed palazzo"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "170097"| "item__name": "sepia brown and white printed cotton top with stripe printed dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -2377,26 +2377,26 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Richi Somani</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>9927354625</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>monicka.sukhija</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>6805</t>
+        </is>
+      </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2023-07-23 16:56:18</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "106956"| "item__name": "sky blue floral printed cotton top with stripe bottom and plain chiffon dupatta"| "visit_count": 1}| {"item__product_id": "169708"| "item__name": "mulberry digital printed chanderi top with brown kantha dupatta se"| "visit_count": 1}| {"item__product_id": "168406"| "item__name": "dark blue digital printed cotton top with dual shade chiffon dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "172422"| "item__name": "black embellished neck work cotton silk top with chanderi dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -2408,78 +2408,82 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shivani </t>
+          <t>Yasmin Shaikh</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>9810198457</t>
+          <t>9370490043</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2023-07-23 18:02:28</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "130325"| "item__name": "neon green south cotton top with magenta mangalgiri hem with dupatta"| "visit_count": 5}| {"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "130943"| "item__name": "Raisin Purple Velvet Top and Brocade Bottom Set"| "visit_count": 4}| {"item__product_id": "148544"| "item__name": "ivory georgette chikankari work 3 piece set with chiffon dupatta"| "visit_count": 3}| {"item__product_id": "164768"| "item__name": "ivory south cotton with mangalgiri hem with midnight blue dupatta set"| "visit_count": 2}| {"item__product_id": "179502"| "item__name": "Blush Pink Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "178613"| "item__name": "baby pink thread work georgette top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "180386"| "item__name": "Maroon Kalamkari Printed Cotton Top with Dobby Work Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182833"| "item__name": "Ruhi Purple Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "177177"| "item__name": "baby blue chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "115461"| "item__name": "Basil Green South Cotton Top with Mangalgiri Hem with Barn Red Dupatta"| "visit_count": 1}| {"item__product_id": "182962"| "item__name": "Barbie World Pink French Knot Cotton Top with Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}]</t>
+          <t>[{"item__product_id": "182962"| "item__name": "Barbie World Pink French Knot Cotton Top with Chiffon Dupatta Set"}| {"item__product_id": "159525"| "item__name": "light orange south cotton top with mangalgiri hem with barn red dupatta"}| {"item__product_id": "181993"| "item__name": "White Cotton Cross Stitch Work Top with White Dupatta Set-1.0"}| {"item__product_id": "148544"| "item__name": "ivory georgette chikankari work 3 piece set with chiffon dupatta"}]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Anju Arya</t>
+          <t xml:space="preserve">Shivani </t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>9816341214</t>
+          <t>9810198457</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2023-07-23 18:03:29</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "61618"| "item__name": "Red kurti with beige palazzo set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182962"| "item__name": "Barbie World Pink French Knot Cotton Top with Chiffon Dupatta Set"| "visit_count": 2}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Anita Das</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr"/>
+          <t>Tanaya Ghosh</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>8250729873</t>
+        </is>
+      </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2023-07-23 18:38:02</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "172384"| "item__name": "maroon red kantha cotton top with rust red ajrak printed dupatta set d2"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "130755"| "item__name": "moss green printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -2491,53 +2495,53 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Anuradha Lochab</t>
+          <t>Chitra Moleshri</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>9718180494</t>
+          <t>9096334614</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2023-07-23 19:21:16</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "175447"| "item__name": "cream white base with pink flower printed co ord set"| "visit_count": 1}]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "174906"| "item__name": "cream and pink cotton dobby chikankari kurti"}]</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Tanaya Ghosh</t>
+          <t>Roshni  RANI Debi</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8250729873</t>
+          <t>9437762745</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2023-07-23 19:22:41</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "130755"| "item__name": "moss green printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 2}]</t>
+          <t>[{"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "178586"| "item__name": "Teal Blue Authentic Chikankari Cotton Top with Chiffon Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -2547,55 +2551,55 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Chitra Moleshri</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>9096334614</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>alka.alka</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>6808</t>
+        </is>
+      </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2023-07-23 20:03:44</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "157273"| "item__name": "ebony black chanderi top with kantha highlight printed dupatta set"| "visit_count": 1}| {"item__product_id": "109151"| "item__name": "white applique scallop palazzo trouser"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "174906"| "item__name": "cream and pink cotton dobby chikankari kurti"}]</t>
+          <t>[{"item__product_id": "177072"| "item__name": "Mushroom Grey Chanderi Embroidered Work Top and Dupatta Set"}]</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Roshni  RANI Debi</t>
+          <t>Anjali Katkade</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>9437762745</t>
+          <t>95032244406</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2023-07-23 20:09:20</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "178586"| "item__name": "Teal Blue Authentic Chikankari Cotton Top with Chiffon Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "137057"| "item__name": "light orchid candy stripe printed cotton top with kota hand painted dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -2605,55 +2609,55 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr"/>
-      <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>alka.alka</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>6808</t>
-        </is>
-      </c>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bindu I </t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>9446364104</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2023-07-23 20:15:43</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177072"| "item__name": "Mushroom Grey Chanderi Embroidered Work Top and Dupatta Set"| "visit_count": 2}| {"item__product_id": "157273"| "item__name": "ebony black chanderi top with kantha highlight printed dupatta set"| "visit_count": 1}| {"item__product_id": "109151"| "item__name": "white applique scallop palazzo trouser"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 1}| {"item__product_id": "182686"| "item__name": "Ruhi Mehendi Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182691"| "item__name": "Nihari Mauve Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 1}| {"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182259"| "item__name": "Darling Mulberry Violet Thread Work Muslin Top with Thread Work Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"| "visit_count": 1}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"| "visit_count": 1}| {"item__product_id": "178888"| "item__name": "pumpkin orange batik handloom top with dupatta set d2"| "visit_count": 1}| {"item__product_id": "170114"| "item__name": "mud beige and garnet red printed cotton top with stripe printed dupatta set 2"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177072"| "item__name": "Mushroom Grey Chanderi Embroidered Work Top and Dupatta Set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Anjali Katkade</t>
+          <t>Chilukuri Madhuri</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>95032244406</t>
+          <t>9491680871</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2023-07-23 20:42:47</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "137057"| "item__name": "light orchid candy stripe printed cotton top with kota hand painted dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "179898"| "item__name": "Tea Green Cotton Linen Floral Chikankari Work Kurti"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -2665,140 +2669,140 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bindu I </t>
+          <t>Shama Hussain</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>9446364104</t>
+          <t>9931944116</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2023-07-23 21:13:32</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 1}| {"item__product_id": "182686"| "item__name": "Ruhi Mehendi Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182691"| "item__name": "Nihari Mauve Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 1}| {"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182259"| "item__name": "Darling Mulberry Violet Thread Work Muslin Top with Thread Work Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"| "visit_count": 1}| {"item__product_id": "181872"| "item__name": "China Pink Plain Chanderi Top with Floral Printed Chanderi Dupatta Set"| "visit_count": 1}| {"item__product_id": "178888"| "item__name": "pumpkin orange batik handloom top with dupatta set d2"| "visit_count": 1}| {"item__product_id": "170114"| "item__name": "mud beige and garnet red printed cotton top with stripe printed dupatta set 2"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182731"| "item__name": "Ruhi Mauve Pink Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182163"| "item__name": "Gulab Jamun Eggplant Georgette Top with Leheriya Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "182731"| "item__name": "Ruhi Mauve Pink Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}]</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Chilukuri Madhuri</t>
+          <t>Savia</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>9491680871</t>
+          <t>9880622825</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2023-07-23 21:31:16</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "179898"| "item__name": "Tea Green Cotton Linen Floral Chikankari Work Kurti"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"| "visit_count": 1}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"}| {"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"}| {"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"}]</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Shama Hussain</t>
+          <t>Sameen Akhter</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>9931944116</t>
+          <t>8872800282</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2023-07-23 22:09:58</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182731"| "item__name": "Ruhi Mauve Pink Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"| "visit_count": 1}| {"item__product_id": "182163"| "item__name": "Gulab Jamun Eggplant Georgette Top with Leheriya Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "177019"| "item__name": "blue and white floral chikankari kurti"| "visit_count": 2}| {"item__product_id": "143701"| "item__name": "Black Printed Cotton Fabric- 1"| "visit_count": 2}| {"item__product_id": "180862"| "item__name": "Turmeric Yellow Mahi Silk Brocade Top fabric"| "visit_count": 2}| {"item__product_id": "147600"| "item__name": "purple glazed top with v neck top and trouser 2 piece set"| "visit_count": 1}| {"item__product_id": "119157"| "item__name": "raisin purple dola silk 3 piece set"| "visit_count": 1}| {"item__product_id": "107604"| "item__name": "slime yellow 2 piece set"| "visit_count": 1}| {"item__product_id": "147268"| "item__name": "cream cotton thread buty top with blonde yellow dupatta set"| "visit_count": 1}| {"item__product_id": "106288"| "item__name": "gold yellow zari work panel 3 piece set"| "visit_count": 1}| {"item__product_id": "113040"| "item__name": "pearl white satin with organza dupatta 3 piece set 2"| "visit_count": 1}| {"item__product_id": "181387"| "item__name": "Persian Luxury Plain Silk Fabric"| "visit_count": 1}| {"item__product_id": "162665"| "item__name": "salmon peach printed cotton top with grey printed dupatta set"| "visit_count": 1}| {"item__product_id": "181043"| "item__name": "Maroon Red Printed Cotton fabric"| "visit_count": 1}| {"item__product_id": "170580"| "item__name": "warm beige embroidered organza top with embroidered organza dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182731"| "item__name": "Ruhi Mauve Pink Tussar Chanderi Silk Top with Chanderi Silk Dupatta Set"}| {"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"}]</t>
+          <t>[{"item__product_id": "177019"| "item__name": "blue and white floral chikankari kurti"}| {"item__product_id": "180862"| "item__name": "Turmeric Yellow Mahi Silk Brocade Top fabric"}]</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>Savia</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>9880622825</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>sameen.akhter</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>6809</t>
+        </is>
+      </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2023-07-23 22:25:37</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"| "visit_count": 1}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "177019"| "item__name": "blue and white floral chikankari kurti"| "visit_count": 2}| {"item__product_id": "143701"| "item__name": "Black Printed Cotton Fabric- 1"| "visit_count": 2}| {"item__product_id": "180862"| "item__name": "Turmeric Yellow Mahi Silk Brocade Top fabric"| "visit_count": 2}| {"item__product_id": "147600"| "item__name": "purple glazed top with v neck top and trouser 2 piece set"| "visit_count": 1}| {"item__product_id": "119157"| "item__name": "raisin purple dola silk 3 piece set"| "visit_count": 1}| {"item__product_id": "107604"| "item__name": "slime yellow 2 piece set"| "visit_count": 1}| {"item__product_id": "147268"| "item__name": "cream cotton thread buty top with blonde yellow dupatta set"| "visit_count": 1}| {"item__product_id": "106288"| "item__name": "gold yellow zari work panel 3 piece set"| "visit_count": 1}| {"item__product_id": "113040"| "item__name": "pearl white satin with organza dupatta 3 piece set 2"| "visit_count": 1}| {"item__product_id": "181387"| "item__name": "Persian Luxury Plain Silk Fabric"| "visit_count": 1}| {"item__product_id": "162665"| "item__name": "salmon peach printed cotton top with grey printed dupatta set"| "visit_count": 1}| {"item__product_id": "181043"| "item__name": "Maroon Red Printed Cotton fabric"| "visit_count": 1}| {"item__product_id": "170580"| "item__name": "warm beige embroidered organza top with embroidered organza dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"}| {"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"}| {"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"}]</t>
+          <t>[{"item__product_id": "177019"| "item__name": "blue and white floral chikankari kurti"}| {"item__product_id": "180862"| "item__name": "Turmeric Yellow Mahi Silk Brocade Top fabric"}]</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vijaya Lakshmi </t>
+          <t xml:space="preserve">Dipika </t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>9494338240</t>
+          <t>7838578993</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2023-07-23 22:44:20</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "128988"| "item__name": "mellow yellow printed chanderi top with kantha inspired printed dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "143107"| "item__name": "bubblegum pink printed cotton kurti"| "visit_count": 3}| {"item__product_id": "169708"| "item__name": "mulberry digital printed chanderi top with brown kantha dupatta se"| "visit_count": 1}| {"item__product_id": "177019"| "item__name": "blue and white floral chikankari kurti"| "visit_count": 1}| {"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}| {"item__product_id": "175054"| "item__name": "blue mix color printed cotton chikankari kurti"| "visit_count": 1}| {"item__product_id": "179919"| "item__name": "indigo printed v neck cotton top with printed bottom and dupatta set"| "visit_count": 1}| {"item__product_id": "142912"| "item__name": "mauve kantha printed 2 piece set"| "visit_count": 1}| {"item__product_id": "117097"| "item__name": "mahogany chanderi kantha 3 piece set"| "visit_count": 1}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}| {"item__product_id": "179104"| "item__name": "Sapphire Blue Floral Printed Cotton Top"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -2808,31 +2812,31 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>Sameen Akhter</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>8872800282</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>sunitaanand195@gmail.com.anand</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>6810</t>
+        </is>
+      </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2023-07-23 23:36:33</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177019"| "item__name": "blue and white floral chikankari kurti"| "visit_count": 2}| {"item__product_id": "143701"| "item__name": "Black Printed Cotton Fabric- 1"| "visit_count": 2}| {"item__product_id": "180862"| "item__name": "Turmeric Yellow Mahi Silk Brocade Top fabric"| "visit_count": 2}| {"item__product_id": "147600"| "item__name": "purple glazed top with v neck top and trouser 2 piece set"| "visit_count": 1}| {"item__product_id": "119157"| "item__name": "raisin purple dola silk 3 piece set"| "visit_count": 1}| {"item__product_id": "107604"| "item__name": "slime yellow 2 piece set"| "visit_count": 1}| {"item__product_id": "147268"| "item__name": "cream cotton thread buty top with blonde yellow dupatta set"| "visit_count": 1}| {"item__product_id": "106288"| "item__name": "gold yellow zari work panel 3 piece set"| "visit_count": 1}| {"item__product_id": "113040"| "item__name": "pearl white satin with organza dupatta 3 piece set 2"| "visit_count": 1}| {"item__product_id": "181387"| "item__name": "Persian Luxury Plain Silk Fabric"| "visit_count": 1}| {"item__product_id": "162665"| "item__name": "salmon peach printed cotton top with grey printed dupatta set"| "visit_count": 1}| {"item__product_id": "181043"| "item__name": "Maroon Red Printed Cotton fabric"| "visit_count": 1}| {"item__product_id": "170580"| "item__name": "warm beige embroidered organza top with embroidered organza dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "170806"| "item__name": "persian pink digital printed cotton top with tie dye chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "169708"| "item__name": "mulberry digital printed chanderi top with brown kantha dupatta se"| "visit_count": 1}| {"item__product_id": "169210"| "item__name": "light sky blue digital printed organza top with organza dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177019"| "item__name": "blue and white floral chikankari kurti"}| {"item__product_id": "180862"| "item__name": "Turmeric Yellow Mahi Silk Brocade Top fabric"}]</t>
+          <t>[{"item__product_id": "170806"| "item__name": "persian pink digital printed cotton top with tie dye chiffon dupatta set"}| {"item__product_id": "170806"| "item__name": "persian pink digital printed cotton top with tie dye chiffon dupatta set"}| {"item__product_id": "170806"| "item__name": "persian pink digital printed cotton top with tie dye chiffon dupatta set"}]</t>
         </is>
       </c>
     </row>
@@ -2841,51 +2845,51 @@
       <c r="B84" t="inlineStr"/>
       <c r="C84" t="inlineStr">
         <is>
-          <t>sameen.akhter</t>
+          <t>kajalsharma908614</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>6809</t>
+          <t>6811</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2023-07-24 00:07:52</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177019"| "item__name": "blue and white floral chikankari kurti"| "visit_count": 2}| {"item__product_id": "143701"| "item__name": "Black Printed Cotton Fabric- 1"| "visit_count": 2}| {"item__product_id": "180862"| "item__name": "Turmeric Yellow Mahi Silk Brocade Top fabric"| "visit_count": 2}| {"item__product_id": "147600"| "item__name": "purple glazed top with v neck top and trouser 2 piece set"| "visit_count": 1}| {"item__product_id": "119157"| "item__name": "raisin purple dola silk 3 piece set"| "visit_count": 1}| {"item__product_id": "107604"| "item__name": "slime yellow 2 piece set"| "visit_count": 1}| {"item__product_id": "147268"| "item__name": "cream cotton thread buty top with blonde yellow dupatta set"| "visit_count": 1}| {"item__product_id": "106288"| "item__name": "gold yellow zari work panel 3 piece set"| "visit_count": 1}| {"item__product_id": "113040"| "item__name": "pearl white satin with organza dupatta 3 piece set 2"| "visit_count": 1}| {"item__product_id": "181387"| "item__name": "Persian Luxury Plain Silk Fabric"| "visit_count": 1}| {"item__product_id": "162665"| "item__name": "salmon peach printed cotton top with grey printed dupatta set"| "visit_count": 1}| {"item__product_id": "181043"| "item__name": "Maroon Red Printed Cotton fabric"| "visit_count": 1}| {"item__product_id": "170580"| "item__name": "warm beige embroidered organza top with embroidered organza dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "134102"| "item__name": "rani pink silk top with embellished neck line and banarasi dupatta set"| "visit_count": 4}| {"item__product_id": "179959"| "item__name": "ruby pink embellished neckline muslin top with chanderi silk dupatta set"| "visit_count": 4}| {"item__product_id": "182163"| "item__name": "Gulab Jamun Eggplant Georgette Top with Leheriya Chiffon Dupatta Set"| "visit_count": 2}| {"item__product_id": "171064"| "item__name": "greyish pink embellished neck work chanderi top with hand printed chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "178142"| "item__name": "\u0938\u0941\u0930\u094d\u0916\u093c \u0917\u0941\u0932\u093e\u092c\u0940 Printed Organza Top with Chiffon Gota Work Dupatta Set"| "visit_count": 2}| {"item__product_id": "141899"| "item__name": "rebecca purple floral digital printed organza top with chiffon gota work dupatta"| "visit_count": 1}| {"item__product_id": "182444"| "item__name": "Rang-e-Sharabat Floral V Neck Muslin Top With Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "176578"| "item__name": "sea blue embellished neck work zig zag muslin top with plain muslin dupatta set"| "visit_count": 1}| {"item__product_id": "177833"| "item__name": "dandelion yellow chanderi top and leheriya chanderi silk dupatta set with potli bag"| "visit_count": 1}| {"item__product_id": "179507"| "item__name": "Aqua Blue Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}| {"item__product_id": "107117"| "item__name": "bumblebee yellow zari polka weave dola silk top with red banarasi dupatta set"| "visit_count": 1}| {"item__product_id": "131381"| "item__name": "hot pink silk v neck top with banarasi dupatta set"| "visit_count": 1}| {"item__product_id": "182691"| "item__name": "Nihari Mauve Chanderi Silk Top with Printed Organza  Dupatta Set"| "visit_count": 1}| {"item__product_id": "168364"| "item__name": "ruby pink leheriya muslin embroidered top with plain muslin dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177019"| "item__name": "blue and white floral chikankari kurti"}| {"item__product_id": "180862"| "item__name": "Turmeric Yellow Mahi Silk Brocade Top fabric"}]</t>
+          <t>[{"item__product_id": "134102"| "item__name": "rani pink silk top with embellished neck line and banarasi dupatta set"}| {"item__product_id": "182163"| "item__name": "Gulab Jamun Eggplant Georgette Top with Leheriya Chiffon Dupatta Set"}| {"item__product_id": "141899"| "item__name": "rebecca purple floral digital printed organza top with chiffon gota work dupatta"}| {"item__product_id": "141899"| "item__name": "rebecca purple floral digital printed organza top with chiffon gota work dupatta"}| {"item__product_id": "141899"| "item__name": "rebecca purple floral digital printed organza top with chiffon gota work dupatta"}| {"item__product_id": "179959"| "item__name": "ruby pink embellished neckline muslin top with chanderi silk dupatta set"}| {"item__product_id": "171064"| "item__name": "greyish pink embellished neck work chanderi top with hand printed chiffon dupatta set"}| {"item__product_id": "171064"| "item__name": "greyish pink embellished neck work chanderi top with hand printed chiffon dupatta set"}| {"item__product_id": "178142"| "item__name": "\u0938\u0941\u0930\u094d\u0916\u093c \u0917\u0941\u0932\u093e\u092c\u0940 Printed Organza Top with Chiffon Gota Work Dupatta Set"}| {"item__product_id": "178142"| "item__name": "\u0938\u0941\u0930\u094d\u0916\u093c \u0917\u0941\u0932\u093e\u092c\u0940 Printed Organza Top with Chiffon Gota Work Dupatta Set"}| {"item__product_id": "178142"| "item__name": "\u0938\u0941\u0930\u094d\u0916\u093c \u0917\u0941\u0932\u093e\u092c\u0940 Printed Organza Top with Chiffon Gota Work Dupatta Set"}| {"item__product_id": "134102"| "item__name": "rani pink silk top with embellished neck line and banarasi dupatta set"}| {"item__product_id": "168364"| "item__name": "ruby pink leheriya muslin embroidered top with plain muslin dupatta set"}| {"item__product_id": "168364"| "item__name": "ruby pink leheriya muslin embroidered top with plain muslin dupatta set"}]</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dipika </t>
+          <t>Megha Kathiwala</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7838578993</t>
+          <t>8866114427</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2023-07-24 00:20:12</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "143107"| "item__name": "bubblegum pink printed cotton kurti"| "visit_count": 3}| {"item__product_id": "169708"| "item__name": "mulberry digital printed chanderi top with brown kantha dupatta se"| "visit_count": 1}| {"item__product_id": "177019"| "item__name": "blue and white floral chikankari kurti"| "visit_count": 1}| {"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}| {"item__product_id": "175054"| "item__name": "blue mix color printed cotton chikankari kurti"| "visit_count": 1}| {"item__product_id": "179919"| "item__name": "indigo printed v neck cotton top with printed bottom and dupatta set"| "visit_count": 1}| {"item__product_id": "142912"| "item__name": "mauve kantha printed 2 piece set"| "visit_count": 1}| {"item__product_id": "117097"| "item__name": "mahogany chanderi kantha 3 piece set"| "visit_count": 1}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}| {"item__product_id": "179104"| "item__name": "Sapphire Blue Floral Printed Cotton Top"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -2899,138 +2903,138 @@
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
-          <t>sunitaanand195@gmail.com.anand</t>
+          <t>neerja.bahuguna</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>6810</t>
+          <t>6813</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2023-07-24 00:53:54</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "170806"| "item__name": "persian pink digital printed cotton top with tie dye chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "169708"| "item__name": "mulberry digital printed chanderi top with brown kantha dupatta se"| "visit_count": 1}| {"item__product_id": "169210"| "item__name": "light sky blue digital printed organza top with organza dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "179359"| "item__name": "mauve chikankari work rayon top with palazzo"| "visit_count": 2}| {"item__product_id": "175054"| "item__name": "blue mix color printed cotton chikankari kurti"| "visit_count": 1}| {"item__product_id": "177343"| "item__name": "blush pink floral printed cotton chikankari kurti"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "170806"| "item__name": "persian pink digital printed cotton top with tie dye chiffon dupatta set"}| {"item__product_id": "170806"| "item__name": "persian pink digital printed cotton top with tie dye chiffon dupatta set"}| {"item__product_id": "170806"| "item__name": "persian pink digital printed cotton top with tie dye chiffon dupatta set"}]</t>
+          <t>[{"item__product_id": "179359"| "item__name": "mauve chikankari work rayon top with palazzo"}]</t>
         </is>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr"/>
-      <c r="B87" t="inlineStr"/>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>kajalsharma908614</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>6811</t>
-        </is>
-      </c>
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Sangeeta</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>9873090636</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2023-07-24 01:17:55</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177963"| "item__name": "bright pink georgette leheriya top with leheriya chiffon dupatta set"| "visit_count": 4}| {"item__product_id": "182152"| "item__name": "Gulab Jamun Eggplant Georgette Leheriya Top with Leheriya Chiffon Dupatta Set"| "visit_count": 4}| {"item__product_id": "182444"| "item__name": "Rang-e-Sharabat Floral V Neck Muslin Top With Chiffon Dupatta Set"| "visit_count": 3}| {"item__product_id": "182439"| "item__name": "Mystic Mauvewood Chanderi Top with Hand Painted Chiffon Dupatta Set"| "visit_count": 3}| {"item__product_id": "182163"| "item__name": "Gulab Jamun Eggplant Georgette Top with Leheriya Chiffon Dupatta Set"| "visit_count": 3}| {"item__product_id": "134102"| "item__name": "rani pink silk top with embellished neck line and banarasi dupatta set"| "visit_count": 2}| {"item__product_id": "179959"| "item__name": "ruby pink embellished neckline muslin top with chanderi silk dupatta set"| "visit_count": 2}| {"item__product_id": "171064"| "item__name": "greyish pink embellished neck work chanderi top with hand printed chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "181881"| "item__name": "Mid Night Blue Printed Chanderi Top with French Knot Work Dupatta Set"| "visit_count": 1}| {"item__product_id": "182391"| "item__name": "Mughal Maroon Digital Printed Angrakha Cotton Top with Dual Shade Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "182540"| "item__name": "Barbie Pink Leheriya Printed Lace Work Cotton Top"| "visit_count": 1}| {"item__product_id": "170426"| "item__name": "amber yellow cotton dobby top with stripe print dupatta set"| "visit_count": 1}| {"item__product_id": "178613"| "item__name": "baby pink thread work georgette top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "141899"| "item__name": "rebecca purple floral digital printed organza top with chiffon gota work dupatta"| "visit_count": 1}| {"item__product_id": "176578"| "item__name": "sea blue embellished neck work zig zag muslin top with plain muslin dupatta set"| "visit_count": 1}| {"item__product_id": "177833"| "item__name": "dandelion yellow chanderi top and leheriya chanderi silk dupatta set with potli bag"| "visit_count": 1}| {"item__product_id": "178142"| "item__name": "\u0938\u0941\u0930\u094d\u0916\u093c \u0917\u0941\u0932\u093e\u092c\u0940 Printed Organza Top with Chiffon Gota Work Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "117550"| "item__name": "fuschia pink muslin 3 piece set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182540"| "item__name": "Barbie Pink Leheriya Printed Lace Work Cotton Top"}| {"item__product_id": "182540"| "item__name": "Barbie Pink Leheriya Printed Lace Work Cotton Top"}| {"item__product_id": "177963"| "item__name": "bright pink georgette leheriya top with leheriya chiffon dupatta set"}| {"item__product_id": "182163"| "item__name": "Gulab Jamun Eggplant Georgette Top with Leheriya Chiffon Dupatta Set"}| {"item__product_id": "182152"| "item__name": "Gulab Jamun Eggplant Georgette Leheriya Top with Leheriya Chiffon Dupatta Set"}| {"item__product_id": "182439"| "item__name": "Mystic Mauvewood Chanderi Top with Hand Painted Chiffon Dupatta Set"}| {"item__product_id": "182444"| "item__name": "Rang-e-Sharabat Floral V Neck Muslin Top With Chiffon Dupatta Set"}| {"item__product_id": "134102"| "item__name": "rani pink silk top with embellished neck line and banarasi dupatta set"}| {"item__product_id": "182163"| "item__name": "Gulab Jamun Eggplant Georgette Top with Leheriya Chiffon Dupatta Set"}| {"item__product_id": "141899"| "item__name": "rebecca purple floral digital printed organza top with chiffon gota work dupatta"}| {"item__product_id": "141899"| "item__name": "rebecca purple floral digital printed organza top with chiffon gota work dupatta"}| {"item__product_id": "141899"| "item__name": "rebecca purple floral digital printed organza top with chiffon gota work dupatta"}| {"item__product_id": "179959"| "item__name": "ruby pink embellished neckline muslin top with chanderi silk dupatta set"}| {"item__product_id": "171064"| "item__name": "greyish pink embellished neck work chanderi top with hand printed chiffon dupatta set"}| {"item__product_id": "171064"| "item__name": "greyish pink embellished neck work chanderi top with hand printed chiffon dupatta set"}| {"item__product_id": "178142"| "item__name": "\u0938\u0941\u0930\u094d\u0916\u093c \u0917\u0941\u0932\u093e\u092c\u0940 Printed Organza Top with Chiffon Gota Work Dupatta Set"}| {"item__product_id": "178142"| "item__name": "\u0938\u0941\u0930\u094d\u0916\u093c \u0917\u0941\u0932\u093e\u092c\u0940 Printed Organza Top with Chiffon Gota Work Dupatta Set"}| {"item__product_id": "178142"| "item__name": "\u0938\u0941\u0930\u094d\u0916\u093c \u0917\u0941\u0932\u093e\u092c\u0940 Printed Organza Top with Chiffon Gota Work Dupatta Set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Megha Kathiwala</t>
+          <t xml:space="preserve">Priyaa Tomer </t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>8866114427</t>
+          <t>8076673943</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2023-07-24 02:35:29</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "112916"| "item__name": "french violet french knot top with white chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "159905"| "item__name": "mint green katan staple handloom top and dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "159905"| "item__name": "mint green katan staple handloom top and dupatta set"}]</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr"/>
-      <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>neerja.bahuguna</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>6813</t>
-        </is>
-      </c>
+      <c r="A89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shikha </t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>8299203399</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2023-07-24 05:54:07</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "179359"| "item__name": "mauve chikankari work rayon top with palazzo"| "visit_count": 2}| {"item__product_id": "175054"| "item__name": "blue mix color printed cotton chikankari kurti"| "visit_count": 1}| {"item__product_id": "177343"| "item__name": "blush pink floral printed cotton chikankari kurti"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "152328"| "item__name": "grey base pink printed cotton chikankari 2 piece set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "179359"| "item__name": "mauve chikankari work rayon top with palazzo"}]</t>
+          <t>[{"item__product_id": "152328"| "item__name": "grey base pink printed cotton chikankari 2 piece set"}]</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Sangeeta</t>
+          <t>Lata chandrashekhar Turkar</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>9873090636</t>
+          <t>9404001926</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2023-07-24 06:03:02</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "117550"| "item__name": "fuschia pink muslin 3 piece set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "168415"| "item__name": "spanish orange modal chikankari kurti d1"| "visit_count": 2}| {"item__product_id": "179353"| "item__name": "midnight blue chikankari work rayon top with palazzo"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -3042,82 +3046,82 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t xml:space="preserve">Priyaa Tomer </t>
+          <t>Bela shah</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>8076673943</t>
+          <t>9825277336</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2023-07-24 07:18:04</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "112916"| "item__name": "french violet french knot top with white chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "159905"| "item__name": "mint green katan staple handloom top and dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "159905"| "item__name": "mint green katan staple handloom top and dupatta set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shikha </t>
+          <t xml:space="preserve">Dipti Prasad </t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>8299203399</t>
+          <t>09810975365</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2023-07-24 07:28:04</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "152328"| "item__name": "grey base pink printed cotton chikankari 2 piece set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "166662"| "item__name": "dove greyish purple printed chikankari top with leheriya printed palazzo"| "visit_count": 1}| {"item__product_id": "177343"| "item__name": "blush pink floral printed cotton chikankari kurti"| "visit_count": 1}| {"item__product_id": "182148"| "item__name": "Kesariya Bright Red Georgette Leheriya Top with Leheriya Chiffon Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "152328"| "item__name": "grey base pink printed cotton chikankari 2 piece set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Lata chandrashekhar Turkar</t>
+          <t>Archna Sharma C/o Dr Sanjay Sharma</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>9404001926</t>
+          <t>9736134202</t>
         </is>
       </c>
       <c r="C93" t="inlineStr"/>
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr">
         <is>
-          <t>2023-07-24 07:31:40</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "168415"| "item__name": "spanish orange modal chikankari kurti d1"| "visit_count": 2}| {"item__product_id": "179353"| "item__name": "midnight blue chikankari work rayon top with palazzo"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "173999"| "item__name": "buttermilk yellow digital printed floral chikankari kurti"| "visit_count": 1}| {"item__product_id": "174871"| "item__name": "grapefruit purple printed chikankari top with leheriya printed palazzo"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -3129,24 +3133,20 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Bela shah</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>9825277336</t>
-        </is>
-      </c>
+          <t>Bhuvanakumar Kumar</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr"/>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2023-07-24 07:43:40</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "130325"| "item__name": "neon green south cotton top with magenta mangalgiri hem with dupatta"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -3158,53 +3158,53 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dipti Prasad </t>
+          <t>Anju Sharma</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>09810975365</t>
+          <t>9729089818</t>
         </is>
       </c>
       <c r="C95" t="inlineStr"/>
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2023-07-24 07:44:14</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "166662"| "item__name": "dove greyish purple printed chikankari top with leheriya printed palazzo"| "visit_count": 1}| {"item__product_id": "177343"| "item__name": "blush pink floral printed cotton chikankari kurti"| "visit_count": 1}| {"item__product_id": "182148"| "item__name": "Kesariya Bright Red Georgette Leheriya Top with Leheriya Chiffon Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}| {"item__product_id": "130325"| "item__name": "neon green south cotton top with magenta mangalgiri hem with dupatta"| "visit_count": 1}| {"item__product_id": "182444"| "item__name": "Rang-e-Sharabat Floral V Neck Muslin Top With Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "169146"| "item__name": "ombre yellow and green muslin top with digital print chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "180386"| "item__name": "Maroon Kalamkari Printed Cotton Top with Dobby Work Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "177189"| "item__name": "bright yellow thread neck work crepe top with floral printed chiffon dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "130325"| "item__name": "neon green south cotton top with magenta mangalgiri hem with dupatta"}]</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Archna Sharma C/o Dr Sanjay Sharma</t>
+          <t>Arofajaved Arofajaved</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>9736134202</t>
+          <t>9434266283</t>
         </is>
       </c>
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr">
         <is>
-          <t>2023-07-24 07:54:01</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "173999"| "item__name": "buttermilk yellow digital printed floral chikankari kurti"| "visit_count": 1}| {"item__product_id": "174871"| "item__name": "grapefruit purple printed chikankari top with leheriya printed palazzo"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182375"| "item__name": "Leher Violet Purple Cotton Leheriya Top with Shibori Chiffon Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -3216,20 +3216,24 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Bhuvanakumar Kumar</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr"/>
+          <t xml:space="preserve">Archana </t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>9811605719</t>
+        </is>
+      </c>
       <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr">
         <is>
-          <t>2023-07-24 07:55:32</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "130325"| "item__name": "neon green south cotton top with magenta mangalgiri hem with dupatta"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "166926"| "item__name": "royal mauve floral printed kurti with front buttons"| "visit_count": 3}| {"item__product_id": "170221"| "item__name": "cream and blue printed cotton co ord set"| "visit_count": 1}| {"item__product_id": "177460"| "item__name": "white plain lycra trouser with lace work"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -3241,53 +3245,53 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Anju Sharma</t>
+          <t>Priya Ahuja</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>9729089818</t>
+          <t>9409420539</t>
         </is>
       </c>
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2023-07-24 08:45:51</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182356"| "item__name": "Mohini Mint Green Cross Stitch work Cotton Linen Top and Dupatta Set"| "visit_count": 1}| {"item__product_id": "130325"| "item__name": "neon green south cotton top with magenta mangalgiri hem with dupatta"| "visit_count": 1}| {"item__product_id": "182444"| "item__name": "Rang-e-Sharabat Floral V Neck Muslin Top With Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "169146"| "item__name": "ombre yellow and green muslin top with digital print chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "180386"| "item__name": "Maroon Kalamkari Printed Cotton Top with Dobby Work Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "177189"| "item__name": "bright yellow thread neck work crepe top with floral printed chiffon dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182361"| "item__name": "London Cornflower Stripe Printed Cotton Top with Chiffon Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "130325"| "item__name": "neon green south cotton top with magenta mangalgiri hem with dupatta"}]</t>
+          <t>[{"item__product_id": "182361"| "item__name": "London Cornflower Stripe Printed Cotton Top with Chiffon Dupatta Set"}]</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Arofajaved Arofajaved</t>
+          <t xml:space="preserve">VEENA. JAIN </t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>9434266283</t>
+          <t>7011745163</t>
         </is>
       </c>
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr">
         <is>
-          <t>2023-07-24 08:49:00</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182375"| "item__name": "Leher Violet Purple Cotton Leheriya Top with Shibori Chiffon Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "149636"| "item__name": "orange dual shade south cotton top with jade green dupatta"| "visit_count": 1}| {"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -3299,198 +3303,198 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t xml:space="preserve">Archana </t>
+          <t>Kiran tripathi</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>9811605719</t>
+          <t>7828904571</t>
         </is>
       </c>
       <c r="C100" t="inlineStr"/>
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr">
         <is>
-          <t>2023-07-24 08:52:45</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "166926"| "item__name": "royal mauve floral printed kurti with front buttons"| "visit_count": 3}| {"item__product_id": "170221"| "item__name": "cream and blue printed cotton co ord set"| "visit_count": 1}| {"item__product_id": "177460"| "item__name": "white plain lycra trouser with lace work"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "162223"| "item__name": "cobalt blue step leheriya chikankari kurti"| "visit_count": 3}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"| "visit_count": 2}| {"item__product_id": "177343"| "item__name": "blush pink floral printed cotton chikankari kurti"| "visit_count": 2}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}| {"item__product_id": "150705"| "item__name": "pewter grey floral printed kota chikankari kurti"| "visit_count": 1}| {"item__product_id": "166662"| "item__name": "dove greyish purple printed chikankari top with leheriya printed palazzo"| "visit_count": 1}| {"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 1}| {"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "61172"| "item__name": "8 baby pink bandhani printed kurti"| "visit_count": 1}| {"item__product_id": "183004"| "item__name": "Lahori Maroon Cotton Pakistani Suit with Embroidered Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "136456"| "item__name": "navy blue kantha cotton top with rust red ajrak printed dupatta 3 piece set"| "visit_count": 1}| {"item__product_id": "133621"| "item__name": "white and mauve printed cotton anarkali 3 piece set"| "visit_count": 1}| {"item__product_id": "147381"| "item__name": "light beige mughal printed cotton top and bottom with kota dupatta 3 piece set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "162223"| "item__name": "cobalt blue step leheriya chikankari kurti"}| {"item__product_id": "162223"| "item__name": "cobalt blue step leheriya chikankari kurti"}| {"item__product_id": "136456"| "item__name": "navy blue kantha cotton top with rust red ajrak printed dupatta 3 piece set"}]</t>
         </is>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>Priya Ahuja</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>9409420539</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>arashika1994dhiman</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>6814</t>
+        </is>
+      </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>2023-07-24 09:35:25</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182361"| "item__name": "London Cornflower Stripe Printed Cotton Top with Chiffon Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "177177"| "item__name": "baby blue chikankari work cotton top and dupatta set"| "visit_count": 6}| {"item__product_id": "169146"| "item__name": "ombre yellow and green muslin top with digital print chiffon dupatta set"| "visit_count": 4}| {"item__product_id": "182409"| "item__name": "Laffy Taffy Lavender Embellished Neck Work Organza Top with Organza Printed Dupatta Set"| "visit_count": 2}| {"item__product_id": "179959"| "item__name": "ruby pink embellished neckline muslin top with chanderi silk dupatta set"| "visit_count": 2}| {"item__product_id": "109151"| "item__name": "white applique scallop palazzo trouser"| "visit_count": 1}| {"item__product_id": "173500"| "item__name": "hot pink embellished neck work cotton top with stripe printed chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "179519"| "item__name": "ebony black thread work georgette top with georgette dupatta set"| "visit_count": 1}| {"item__product_id": "169155"| "item__name": "ombre purple and sky blue muslin top with digital print chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"| "visit_count": 1}| {"item__product_id": "171030"| "item__name": "carolina blue dola silk top with embellished neck line and banarasi dupatta set"| "visit_count": 1}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"| "visit_count": 1}| {"item__product_id": "163884"| "item__name": "sandcastle beige printed cotton linen top with printed dupatta set"| "visit_count": 1}| {"item__product_id": "168086"| "item__name": "mulberry mauve digital printed chanderi top with zig zag print dupatta set"| "visit_count": 1}| {"item__product_id": "180403"| "item__name": "Jam Red Applique Work Glazed Cotton Top with Art Chanderi Dupatta Set"| "visit_count": 1}| {"item__product_id": "174896"| "item__name": "jazzberry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "181702"| "item__name": "Ivory White Floral Printed Cotton Top with Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "175262"| "item__name": "tea green kota hand embroidered chikankari top and dupatta 2 piece set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182361"| "item__name": "London Cornflower Stripe Printed Cotton Top with Chiffon Dupatta Set"}]</t>
+          <t>[{"item__product_id": "177177"| "item__name": "baby blue chikankari work cotton top and dupatta set"}| {"item__product_id": "177177"| "item__name": "baby blue chikankari work cotton top and dupatta set"}| {"item__product_id": "169146"| "item__name": "ombre yellow and green muslin top with digital print chiffon dupatta set"}| {"item__product_id": "168086"| "item__name": "mulberry mauve digital printed chanderi top with zig zag print dupatta set"}| {"item__product_id": "179959"| "item__name": "ruby pink embellished neckline muslin top with chanderi silk dupatta set"}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"}| {"item__product_id": "177177"| "item__name": "baby blue chikankari work cotton top and dupatta set"}]</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t xml:space="preserve">VEENA. JAIN </t>
+          <t xml:space="preserve">Mausumi Ghosh Dastidar </t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>7011745163</t>
+          <t>8777267857</t>
         </is>
       </c>
       <c r="C102" t="inlineStr"/>
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr">
         <is>
-          <t>2023-07-24 09:49:58</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "149636"| "item__name": "orange dual shade south cotton top with jade green dupatta"| "visit_count": 1}| {"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182037"| "item__name": "Ruhani Red Dark Green Ajrak Printed Cotton Top With Block Printed Kota Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "182037"| "item__name": "Ruhani Red Dark Green Ajrak Printed Cotton Top With Block Printed Kota Dupatta Set"}]</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Kiran tripathi</t>
+          <t xml:space="preserve">Poorna Shankar </t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>7828904571</t>
+          <t>8447718622</t>
         </is>
       </c>
       <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr">
         <is>
-          <t>2023-07-24 10:37:03</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "162223"| "item__name": "cobalt blue step leheriya chikankari kurti"| "visit_count": 3}| {"item__product_id": "177343"| "item__name": "blush pink floral printed cotton chikankari kurti"| "visit_count": 2}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"| "visit_count": 1}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}| {"item__product_id": "150705"| "item__name": "pewter grey floral printed kota chikankari kurti"| "visit_count": 1}| {"item__product_id": "166662"| "item__name": "dove greyish purple printed chikankari top with leheriya printed palazzo"| "visit_count": 1}| {"item__product_id": "182458"| "item__name": "Mahogany Chanderi Kantha 3 Piece Set"| "visit_count": 1}| {"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "137550"| "item__name": "offwhite and sage green 3 piece set with chiffon digital printed dupatta"| "visit_count": 1}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"| "visit_count": 1}| {"item__product_id": "165655"| "item__name": "cream and sea green printed cotton fabric"| "visit_count": 1}| {"item__product_id": "154520"| "item__name": "light pink art cotton co ord set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "162223"| "item__name": "cobalt blue step leheriya chikankari kurti"}| {"item__product_id": "162223"| "item__name": "cobalt blue step leheriya chikankari kurti"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr"/>
-      <c r="B104" t="inlineStr"/>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>arashika1994dhiman</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>6814</t>
-        </is>
-      </c>
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Ragini Nigam</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>9911070457</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr">
         <is>
-          <t>2023-07-24 10:37:31</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177177"| "item__name": "baby blue chikankari work cotton top and dupatta set"| "visit_count": 6}| {"item__product_id": "169146"| "item__name": "ombre yellow and green muslin top with digital print chiffon dupatta set"| "visit_count": 4}| {"item__product_id": "182409"| "item__name": "Laffy Taffy Lavender Embellished Neck Work Organza Top with Organza Printed Dupatta Set"| "visit_count": 2}| {"item__product_id": "179959"| "item__name": "ruby pink embellished neckline muslin top with chanderi silk dupatta set"| "visit_count": 2}| {"item__product_id": "175262"| "item__name": "tea green kota hand embroidered chikankari top and dupatta 2 piece set"| "visit_count": 1}| {"item__product_id": "181702"| "item__name": "Ivory White Floral Printed Cotton Top with Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "174896"| "item__name": "jazzberry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "180403"| "item__name": "Jam Red Applique Work Glazed Cotton Top with Art Chanderi Dupatta Set"| "visit_count": 1}| {"item__product_id": "168086"| "item__name": "mulberry mauve digital printed chanderi top with zig zag print dupatta set"| "visit_count": 1}| {"item__product_id": "163884"| "item__name": "sandcastle beige printed cotton linen top with printed dupatta set"| "visit_count": 1}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"| "visit_count": 1}| {"item__product_id": "171030"| "item__name": "carolina blue dola silk top with embellished neck line and banarasi dupatta set"| "visit_count": 1}| {"item__product_id": "160787"| "item__name": "olive green chanderi top with madhubani kantha dupatta set"| "visit_count": 1}| {"item__product_id": "169155"| "item__name": "ombre purple and sky blue muslin top with digital print chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "179519"| "item__name": "ebony black thread work georgette top with georgette dupatta set"| "visit_count": 1}| {"item__product_id": "173500"| "item__name": "hot pink embellished neck work cotton top with stripe printed chiffon dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "61618"| "item__name": "Red kurti with beige palazzo set"| "visit_count": 1}| {"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}| {"item__product_id": "150705"| "item__name": "pewter grey floral printed kota chikankari kurti"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177177"| "item__name": "baby blue chikankari work cotton top and dupatta set"}| {"item__product_id": "177177"| "item__name": "baby blue chikankari work cotton top and dupatta set"}| {"item__product_id": "169146"| "item__name": "ombre yellow and green muslin top with digital print chiffon dupatta set"}| {"item__product_id": "168086"| "item__name": "mulberry mauve digital printed chanderi top with zig zag print dupatta set"}| {"item__product_id": "179959"| "item__name": "ruby pink embellished neckline muslin top with chanderi silk dupatta set"}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mausumi Ghosh Dastidar </t>
+          <t xml:space="preserve">Deepa T Unnikrishnan </t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>8777267857</t>
+          <t>9447111542</t>
         </is>
       </c>
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr">
         <is>
-          <t>2023-07-24 11:19:20</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182037"| "item__name": "Ruhani Red Dark Green Ajrak Printed Cotton Top With Block Printed Kota Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182037"| "item__name": "Ruhani Red Dark Green Ajrak Printed Cotton Top With Block Printed Kota Dupatta Set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poorna Shankar </t>
+          <t>Ruhi garg Garg</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>8447718622</t>
+          <t>8837572105</t>
         </is>
       </c>
       <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr">
         <is>
-          <t>2023-07-24 11:19:29</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "137550"| "item__name": "offwhite and sage green 3 piece set with chiffon digital printed dupatta"| "visit_count": 1}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}| {"item__product_id": "167082"| "item__name": "helio purple printed cotton fabric with schiffli fabric"| "visit_count": 1}| {"item__product_id": "165655"| "item__name": "cream and sea green printed cotton fabric"| "visit_count": 1}| {"item__product_id": "154520"| "item__name": "light pink art cotton co ord set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "178613"| "item__name": "baby pink thread work georgette top with chiffon dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -3502,24 +3506,24 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Ragini Nigam</t>
+          <t xml:space="preserve">Madhu </t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>9911070457</t>
+          <t>9717989684</t>
         </is>
       </c>
       <c r="C107" t="inlineStr"/>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr">
         <is>
-          <t>2023-07-24 11:32:08</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "61618"| "item__name": "Red kurti with beige palazzo set"| "visit_count": 1}| {"item__product_id": "96007"| "item__name": "black straight fit kurti"| "visit_count": 1}| {"item__product_id": "150705"| "item__name": "pewter grey floral printed kota chikankari kurti"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "137550"| "item__name": "offwhite and sage green 3 piece set with chiffon digital printed dupatta"| "visit_count": 1}| {"item__product_id": "61618"| "item__name": "Red kurti with beige palazzo set"| "visit_count": 1}| {"item__product_id": "150705"| "item__name": "pewter grey floral printed kota chikankari kurti"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -3531,24 +3535,24 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t xml:space="preserve">Deepa T Unnikrishnan </t>
+          <t>Ranjeeta</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>9447111542</t>
+          <t>6360658568</t>
         </is>
       </c>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr">
         <is>
-          <t>2023-07-24 11:41:23</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "162809"| "item__name": "ivory hakoba work cotton dress with belt"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "137550"| "item__name": "offwhite and sage green 3 piece set with chiffon digital printed dupatta"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -3560,24 +3564,24 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Ruhi garg Garg</t>
+          <t>Uma myneni</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>8837572105</t>
+          <t>9441284747</t>
         </is>
       </c>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr">
         <is>
-          <t>2023-07-24 11:53:14</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "178613"| "item__name": "baby pink thread work georgette top with chiffon dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "175558"| "item__name": "buttermilk yellow digital printed floral chikankari kurti d2"| "visit_count": 2}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}| {"item__product_id": "117527"| "item__name": "crimson pink muslin 3 piece garara set"| "visit_count": 1}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"| "visit_count": 1}| {"item__product_id": "104294"| "item__name": "black mushru 3 piece set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -3587,84 +3591,84 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Madhu </t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>9717989684</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr"/>
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>monika.sharma</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>6815</t>
+        </is>
+      </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>2023-07-24 11:53:56</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "137550"| "item__name": "offwhite and sage green 3 piece set with chiffon digital printed dupatta"| "visit_count": 1}| {"item__product_id": "61618"| "item__name": "Red kurti with beige palazzo set"| "visit_count": 1}| {"item__product_id": "150705"| "item__name": "pewter grey floral printed kota chikankari kurti"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "177181"| "item__name": "baby pink chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "182300"| "item__name": "Nawabi Mint Green Authentic Chikankari Cotton Top with Cotton Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "177181"| "item__name": "baby pink chikankari work cotton top and dupatta set"}]</t>
         </is>
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>Ranjeeta</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>6360658568</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr"/>
-      <c r="D111" t="inlineStr"/>
+      <c r="A111" t="inlineStr"/>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>dr.sukritapaul</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>6816</t>
+        </is>
+      </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>2023-07-24 11:55:34</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "137550"| "item__name": "offwhite and sage green 3 piece set with chiffon digital printed dupatta"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"| "visit_count": 3}| {"item__product_id": "148501"| "item__name": "off white printed cotton linen with chiffon dupatta 3 piece set"| "visit_count": 2}| {"item__product_id": "148536"| "item__name": "slime green muslin 3 piece set with organza dupatta"| "visit_count": 2}| {"item__product_id": "171768"| "item__name": "black floral designer neck work muslin top with organza dupatta set"| "visit_count": 1}| {"item__product_id": "168581"| "item__name": "sage green digital printed muslin 3 piece set with beautiful lace work dupatta"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{"item__product_id": "148501"| "item__name": "off white printed cotton linen with chiffon dupatta 3 piece set"}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"}| {"item__product_id": "171768"| "item__name": "black floral designer neck work muslin top with organza dupatta set"}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"}| {"item__product_id": "148501"| "item__name": "off white printed cotton linen with chiffon dupatta 3 piece set"}| {"item__product_id": "148536"| "item__name": "slime green muslin 3 piece set with organza dupatta"}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"}]</t>
         </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>Uma myneni</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>9441284747</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr"/>
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>mridulazha</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>6817</t>
+        </is>
+      </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>2023-07-24 12:12:49</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "175558"| "item__name": "buttermilk yellow digital printed floral chikankari kurti d2"| "visit_count": 2}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}| {"item__product_id": "117527"| "item__name": "crimson pink muslin 3 piece garara set"| "visit_count": 1}| {"item__product_id": "171019"| "item__name": "mustard yellow chanderi embroidered work top and dupatta set"| "visit_count": 1}| {"item__product_id": "104294"| "item__name": "black mushru 3 piece set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "179529"| "item__name": "Light Blue Floral Embroidered Neck Work with Sequence Work Chiffon Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -3674,31 +3678,31 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr"/>
-      <c r="B113" t="inlineStr"/>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>monika.sharma</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>6815</t>
-        </is>
-      </c>
+      <c r="A113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anita </t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>7873600262</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr">
         <is>
-          <t>2023-07-24 12:29:36</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "167519"| "item__name": "cherry pink authentic chikankari cotton top with chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "177181"| "item__name": "baby pink chikankari work cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "182300"| "item__name": "Nawabi Mint Green Authentic Chikankari Cotton Top with Cotton Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "170426"| "item__name": "amber yellow cotton dobby top with stripe print dupatta set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "177181"| "item__name": "baby pink chikankari work cotton top and dupatta set"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -3707,51 +3711,51 @@
       <c r="B114" t="inlineStr"/>
       <c r="C114" t="inlineStr">
         <is>
-          <t>dr.sukritapaul</t>
+          <t>prernaps</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>6816</t>
+          <t>6818</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>2023-07-24 13:23:38</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"| "visit_count": 3}| {"item__product_id": "148501"| "item__name": "off white printed cotton linen with chiffon dupatta 3 piece set"| "visit_count": 2}| {"item__product_id": "148536"| "item__name": "slime green muslin 3 piece set with organza dupatta"| "visit_count": 2}| {"item__product_id": "171768"| "item__name": "black floral designer neck work muslin top with organza dupatta set"| "visit_count": 1}| {"item__product_id": "168581"| "item__name": "sage green digital printed muslin 3 piece set with beautiful lace work dupatta"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}| {"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 1}| {"item__product_id": "182892"| "item__name": "Coca Cola Black Kantha Work Cotton Top with Chanderi Dupatta Set"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "148501"| "item__name": "off white printed cotton linen with chiffon dupatta 3 piece set"}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"}| {"item__product_id": "171768"| "item__name": "black floral designer neck work muslin top with organza dupatta set"}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"}| {"item__product_id": "148501"| "item__name": "off white printed cotton linen with chiffon dupatta 3 piece set"}| {"item__product_id": "148536"| "item__name": "slime green muslin 3 piece set with organza dupatta"}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr"/>
-      <c r="B115" t="inlineStr"/>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>mridulazha</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>6817</t>
-        </is>
-      </c>
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Matilda Sanjay Almeida Almeida</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>7021123155</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr">
         <is>
-          <t>2023-07-24 13:31:38</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "179529"| "item__name": "Light Blue Floral Embroidered Neck Work with Sequence Work Chiffon Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "179353"| "item__name": "midnight blue chikankari work rayon top with palazzo"| "visit_count": 2}]</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -3763,24 +3767,24 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t xml:space="preserve">Anita </t>
+          <t xml:space="preserve">Prabha Mishra </t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>7873600262</t>
+          <t>9582455961</t>
         </is>
       </c>
       <c r="C116" t="inlineStr"/>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr">
         <is>
-          <t>2023-07-24 13:52:32</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "179654"| "item__name": "bright pink leheriya printed cotton top with shibori printed cotton dupatta set"| "visit_count": 1}| {"item__product_id": "170426"| "item__name": "amber yellow cotton dobby top with stripe print dupatta set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "169685"| "item__name": "midnight blue digital printed top with kantha dupatta set 2"| "visit_count": 2}]</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -3790,31 +3794,288 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr"/>
-      <c r="B117" t="inlineStr"/>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>prernaps</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>6818</t>
-        </is>
-      </c>
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Ruchi Shankhdhar</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>8077933954</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr">
         <is>
-          <t>2023-07-24 14:05:40</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>[{"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 1}]</t>
+          <t>[{"item__product_id": "172717"| "item__name": "black and white modal chikankari kurti"| "visit_count": 1}]</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
           <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Anju jaiswal</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>9969223655</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>2023-07-24</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "137550"| "item__name": "offwhite and sage green 3 piece set with chiffon digital printed dupatta"| "visit_count": 1}| {"item__product_id": "182385"| "item__name": "Leher Turquoise Blue Cotton Leheriya Top with Patra Work Chiffon Dupatta Set"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr"/>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>kavisha.sengupta</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>6820</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>2023-07-24</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "145469"| "item__name": "white and pink floral printed cotton top and dupatta set"| "visit_count": 1}| {"item__product_id": "143740"| "item__name": "cream printed cotton fabric 2 piece"| "visit_count": 1}| {"item__product_id": "170868"| "item__name": "flamingo pink embroidered linen top with bird embroidered linen dupatta set"| "visit_count": 1}| {"item__product_id": "181409"| "item__name": "Maroon Wine Embroidered Glazed Cotton fabric"| "visit_count": 1}| {"item__product_id": "180555"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nupur Mukherji </t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>9051126972</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr"/>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>2023-07-24</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "166926"| "item__name": "royal mauve floral printed kurti with front buttons"| "visit_count": 1}| {"item__product_id": "180555"| "item__name": "Lilac Thread Work Kota Doriya Top with Thread Work Dupatta Set-D2"| "visit_count": 1}| {"item__product_id": "88427"| "item__name": "tulip pink thread work cotton 3 piece set"| "visit_count": 1}| {"item__product_id": "61618"| "item__name": "Red kurti with beige palazzo set"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Rosalin Mishra</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>7016212230</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>2023-07-24</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "150697"| "item__name": "lemon yellow floral printed kota chikankari kurti"| "visit_count": 1}| {"item__product_id": "179514"| "item__name": "beige embellished neckline chanderi top with floral printed organza dupatta set"| "visit_count": 1}| {"item__product_id": "162669"| "item__name": "blond yellow printed cotton top with grey printed dupatta set"| "visit_count": 1}| {"item__product_id": "179502"| "item__name": "Blush Pink Thread Work Chanderi Top with Printed Organza Dupatta Set"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Minocha Seema</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr"/>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>2023-07-24</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "174906"| "item__name": "cream and pink cotton dobby chikankari kurti"| "visit_count": 1}| {"item__product_id": "175082"| "item__name": "light lilac modal chikankari kurti"| "visit_count": 1}| {"item__product_id": "174871"| "item__name": "grapefruit purple printed chikankari top with leheriya printed palazzo"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Rekha gupta</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>9910082424</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>2023-07-24</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "138018"| "item__name": "maroon kantha cotton top with black ajrak printed dupatta 3 piece set"| "visit_count": 5}| {"item__product_id": "168530"| "item__name": "Light Olive Green Muslin 3 Piece Set with Organza Dupatta"| "visit_count": 1}| {"item__product_id": "117527"| "item__name": "crimson pink muslin 3 piece garara set"| "visit_count": 1}| {"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"| "visit_count": 1}| {"item__product_id": "170185"| "item__name": "black cotton flex top with lace work 2 piece set"| "visit_count": 1}| {"item__product_id": "136467"| "item__name": "Mustard Yellow Kantha Cotton Top with Rust Red Ajrak Printed Dupatta 3 Piece Set"| "visit_count": 1}| {"item__product_id": "152231"| "item__name": "navy blue straight fit kurti"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "182600"| "item__name": "Madhubala Pink leheriya Printed Cotton 2 Piece Set"}| {"item__product_id": "138018"| "item__name": "maroon kantha cotton top with black ajrak printed dupatta 3 piece set"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Muni</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>9704019997</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>2023-07-24</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "61172"| "item__name": "8 baby pink bandhani printed kurti"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr"/>
+      <c r="B125" t="inlineStr"/>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>navjot.sandhu</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>6821</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>2023-07-24</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "172321"| "item__name": "beige and blue digital printed linen top with chiffon dupatta set"| "visit_count": 3}| {"item__product_id": "175424"| "item__name": "wine authentic chikankari ikkat top"| "visit_count": 2}| {"item__product_id": "173694"| "item__name": "black printed v neck cotton top with semi georgette and cotton dupatta set d2"| "visit_count": 2}| {"item__product_id": "176593"| "item__name": "sangria floral printed cotton linen with cotton linen dupatta set"| "visit_count": 2}| {"item__product_id": "145123"| "item__name": "fog grey zig zag digital printed muslin top with chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "145124"| "item__name": "greenish yellow zig zag digital printed muslin top with chiffon dupatta set"| "visit_count": 2}| {"item__product_id": "178613"| "item__name": "baby pink thread work georgette top with chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "171768"| "item__name": "black floral designer neck work muslin top with organza dupatta set"| "visit_count": 1}| {"item__product_id": "168382"| "item__name": "black printed cotton top with semi georgette and cotton dupatta set"| "visit_count": 1}| {"item__product_id": "175651"| "item__name": "cosmic yellow hand parsi embroidered chikankari with mukesh work top"| "visit_count": 1}| {"item__product_id": "174178"| "item__name": "eggplant purple embellished neck work silk top with banarasi dupatta set"| "visit_count": 1}| {"item__product_id": "170992"| "item__name": "creamy white crochet work pakistani suit with floral chiffon dupatta set"| "visit_count": 1}| {"item__product_id": "109151"| "item__name": "white applique scallop palazzo trouser"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "168382"| "item__name": "black printed cotton top with semi georgette and cotton dupatta set"}| {"item__product_id": "176593"| "item__name": "sangria floral printed cotton linen with cotton linen dupatta set"}| {"item__product_id": "176593"| "item__name": "sangria floral printed cotton linen with cotton linen dupatta set"}| {"item__product_id": "172321"| "item__name": "beige and blue digital printed linen top with chiffon dupatta set"}| {"item__product_id": "109151"| "item__name": "white applique scallop palazzo trouser"}| {"item__product_id": "145123"| "item__name": "fog grey zig zag digital printed muslin top with chiffon dupatta set"}| {"item__product_id": "145124"| "item__name": "greenish yellow zig zag digital printed muslin top with chiffon dupatta set"}| {"item__product_id": "173694"| "item__name": "black printed v neck cotton top with semi georgette and cotton dupatta set d2"}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Kalpana Chawla</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>9873376297</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>2023-07-24</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "182168"| "item__name": "Berry Berry Mauve Cotton Top with Shibori Printed Chiffon Dupatta Set"| "visit_count": 2}| {"item__product_id": "180191"| "item__name": "Beige Ikkat Printed Khadi Cotton Top with Forest Green Cotton  Dupatta Set"| "visit_count": 1}]</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>[{"item__product_id": "180191"| "item__name": "Beige Ikkat Printed Khadi Cotton Top with Forest Green Cotton  Dupatta Set"}| {"item__product_id": "180191"| "item__name": "Beige Ikkat Printed Khadi Cotton Top with Forest Green Cotton  Dupatta Set"}]</t>
         </is>
       </c>
     </row>

</xml_diff>